<commit_message>
bug fix for datetime
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="90">
   <si>
     <t>frames</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>old fps</t>
-  </si>
-  <si>
-    <t>length (datetime)</t>
   </si>
   <si>
     <t>ID</t>
@@ -345,12 +342,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,27 +641,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -676,25 +672,22 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>2146</v>
@@ -705,17 +698,14 @@
       <c r="H2">
         <v>29.37533058368741</v>
       </c>
-      <c r="I2" s="2">
-        <v>0.0008455381597222222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>1138</v>
@@ -726,21 +716,18 @@
       <c r="H3">
         <v>29.48353041700283</v>
       </c>
-      <c r="I3" s="2">
-        <v>0.0004467340277777778</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4">
         <v>143</v>
@@ -751,17 +738,14 @@
       <c r="H4">
         <v>18.5637740282416</v>
       </c>
-      <c r="I4" s="2">
-        <v>8.915711805555555E-05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5">
         <v>1137</v>
@@ -772,21 +756,18 @@
       <c r="H5">
         <v>29.77172003428592</v>
       </c>
-      <c r="I5" s="2">
-        <v>0.0004420208912037037</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>1790</v>
@@ -797,21 +778,18 @@
       <c r="H6">
         <v>49.56553180797393</v>
       </c>
-      <c r="I6" s="2">
-        <v>0.0004179838657407407</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>3872</v>
@@ -822,23 +800,20 @@
       <c r="H7">
         <v>53.74154701816303</v>
       </c>
-      <c r="I7" s="2">
-        <v>0.000833895138888889</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>1340</v>
@@ -849,21 +824,18 @@
       <c r="H8">
         <v>36.15796475774919</v>
       </c>
-      <c r="I8" s="2">
-        <v>0.0004289306481481481</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9">
         <v>1398</v>
@@ -874,21 +846,18 @@
       <c r="H9">
         <v>33.84182245040358</v>
       </c>
-      <c r="I9" s="2">
-        <v>0.0004781230555555555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>1438</v>
@@ -899,21 +868,18 @@
       <c r="H10">
         <v>55.38997624779211</v>
       </c>
-      <c r="I10" s="2">
-        <v>0.0003004788888888889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11">
         <v>1470</v>
@@ -924,25 +890,22 @@
       <c r="H11">
         <v>55.33022186779095</v>
       </c>
-      <c r="I11" s="2">
-        <v>0.0003074972106481481</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>2582</v>
@@ -953,21 +916,18 @@
       <c r="H12">
         <v>52.77682440866399</v>
       </c>
-      <c r="I12" s="2">
-        <v>0.0005662382986111111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13">
         <v>3145</v>
@@ -978,21 +938,18 @@
       <c r="H13">
         <v>51.74048067284933</v>
       </c>
-      <c r="I13" s="2">
-        <v>0.00070352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>2578</v>
@@ -1003,21 +960,18 @@
       <c r="H14">
         <v>41.80165455424</v>
       </c>
-      <c r="I14" s="2">
-        <v>0.0007137986111111111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>2704</v>
@@ -1028,23 +982,20 @@
       <c r="H15">
         <v>42.3832389964044</v>
       </c>
-      <c r="I15" s="2">
-        <v>0.0007384120949074074</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16">
         <v>1188</v>
@@ -1055,21 +1006,18 @@
       <c r="H16">
         <v>45.12532019320474</v>
       </c>
-      <c r="I16" s="2">
-        <v>0.0003047069791666667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17">
         <v>1279</v>
@@ -1080,21 +1028,18 @@
       <c r="H17">
         <v>43.65841844563059</v>
       </c>
-      <c r="I17" s="2">
-        <v>0.0003390695601851852</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18">
         <v>1406</v>
@@ -1105,21 +1050,18 @@
       <c r="H18">
         <v>55.64724333807311</v>
       </c>
-      <c r="I18" s="2">
-        <v>0.0002924340393518519</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19">
         <v>1335</v>
@@ -1130,25 +1072,22 @@
       <c r="H19">
         <v>54.24535307284484</v>
       </c>
-      <c r="I19" s="2">
-        <v>0.0002848426273148148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20">
         <v>2495</v>
@@ -1159,21 +1098,18 @@
       <c r="H20">
         <v>43.806707739274</v>
       </c>
-      <c r="I20" s="2">
-        <v>0.0006591984722222222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21">
         <v>2501</v>
@@ -1184,21 +1120,18 @@
       <c r="H21">
         <v>43.65041833803467</v>
       </c>
-      <c r="I21" s="2">
-        <v>0.0006631496412037037</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22">
         <v>2656</v>
@@ -1209,21 +1142,18 @@
       <c r="H22">
         <v>55.17562301089387</v>
       </c>
-      <c r="I22" s="2">
-        <v>0.0005571435185185186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23">
         <v>2686</v>
@@ -1234,23 +1164,20 @@
       <c r="H23">
         <v>54.9289364553392</v>
       </c>
-      <c r="I23" s="2">
-        <v>0.0005659669560185186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24">
         <v>1506</v>
@@ -1261,21 +1188,18 @@
       <c r="H24">
         <v>54.08503827198805</v>
       </c>
-      <c r="I24" s="2">
-        <v>0.0003222805439814815</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F25">
         <v>1540</v>
@@ -1286,21 +1210,18 @@
       <c r="H25">
         <v>52.08371381500893</v>
       </c>
-      <c r="I25" s="2">
-        <v>0.0003422197222222222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26">
         <v>1519</v>
@@ -1311,21 +1232,18 @@
       <c r="H26">
         <v>51.67285686400935</v>
       </c>
-      <c r="I26" s="2">
-        <v>0.0003402370138888889</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27">
         <v>1487</v>
@@ -1336,25 +1254,22 @@
       <c r="H27">
         <v>47.54146978146526</v>
       </c>
-      <c r="I27" s="2">
-        <v>0.0003620133796296296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28">
         <v>1682</v>
@@ -1365,21 +1280,18 @@
       <c r="H28">
         <v>53.15272110331144</v>
       </c>
-      <c r="I28" s="2">
-        <v>0.0003662576851851852</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29">
         <v>1457</v>
@@ -1390,21 +1302,18 @@
       <c r="H29">
         <v>51.93292974401343</v>
       </c>
-      <c r="I29" s="2">
-        <v>0.000324715474537037</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F30">
         <v>1511</v>
@@ -1415,21 +1324,18 @@
       <c r="H30">
         <v>49.68259365892278</v>
       </c>
-      <c r="I30" s="2">
-        <v>0.0003520030787037037</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31">
         <v>3665</v>
@@ -1440,23 +1346,20 @@
       <c r="H31">
         <v>47.33297722747829</v>
       </c>
-      <c r="I31" s="2">
-        <v>0.0008961824074074074</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32">
         <v>1537</v>
@@ -1467,21 +1370,18 @@
       <c r="H32">
         <v>41.48374145021978</v>
       </c>
-      <c r="I32" s="2">
-        <v>0.0004288270833333333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33">
         <v>1563</v>
@@ -1492,21 +1392,18 @@
       <c r="H33">
         <v>42.34418835496892</v>
       </c>
-      <c r="I33" s="2">
-        <v>0.000427219849537037</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F34">
         <v>1867</v>
@@ -1517,21 +1414,18 @@
       <c r="H34">
         <v>40.9332222165535</v>
       </c>
-      <c r="I34" s="2">
-        <v>0.0005279036226851851</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F35">
         <v>3217</v>
@@ -1542,25 +1436,22 @@
       <c r="H35">
         <v>42.92150128390925</v>
       </c>
-      <c r="I35" s="2">
-        <v>0.0008674858796296295</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36">
         <v>1830</v>
@@ -1571,21 +1462,18 @@
       <c r="H36">
         <v>49.70247365952225</v>
       </c>
-      <c r="I36" s="2">
-        <v>0.0004261469097222223</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37">
         <v>2103</v>
@@ -1596,21 +1484,18 @@
       <c r="H37">
         <v>53.70913964828354</v>
       </c>
-      <c r="I37" s="2">
-        <v>0.000453186886574074</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F38">
         <v>2176</v>
@@ -1621,21 +1506,18 @@
       <c r="H38">
         <v>47.66397980694467</v>
       </c>
-      <c r="I38" s="2">
-        <v>0.0005283903125000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39">
         <v>1909</v>
@@ -1646,25 +1528,22 @@
       <c r="H39">
         <v>47.5207439622642</v>
       </c>
-      <c r="I39" s="2">
-        <v>0.0004649528935185185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F40">
         <v>1536</v>
@@ -1675,17 +1554,14 @@
       <c r="H40">
         <v>56.15083400804507</v>
       </c>
-      <c r="I40" s="2">
-        <v>0.0003166075462962963</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F41">
         <v>1413</v>
@@ -1696,17 +1572,14 @@
       <c r="H41">
         <v>52.1457380749469</v>
       </c>
-      <c r="I41" s="2">
-        <v>0.0003136242245370371</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42">
         <v>1420</v>
@@ -1717,21 +1590,18 @@
       <c r="H42">
         <v>51.41623111929007</v>
       </c>
-      <c r="I42" s="2">
-        <v>0.0003196497453703704</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43">
         <v>1460</v>
@@ -1742,21 +1612,18 @@
       <c r="H43">
         <v>54.28122126650507</v>
       </c>
-      <c r="I43" s="2">
-        <v>0.0003113074421296296</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F44">
         <v>1564</v>
@@ -1767,21 +1634,18 @@
       <c r="H44">
         <v>54.92985240095786</v>
       </c>
-      <c r="I44" s="2">
-        <v>0.0003295448842592592</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F45">
         <v>1713</v>
@@ -1792,25 +1656,22 @@
       <c r="H45">
         <v>55.18471868454063</v>
       </c>
-      <c r="I45" s="2">
-        <v>0.0003592731712962963</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F46">
         <v>1997</v>
@@ -1821,21 +1682,18 @@
       <c r="H46">
         <v>46.77091999195924</v>
       </c>
-      <c r="I46" s="2">
-        <v>0.0004941836921296296</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F47">
         <v>2311</v>
@@ -1846,21 +1704,18 @@
       <c r="H47">
         <v>44.82867396394455</v>
       </c>
-      <c r="I47" s="2">
-        <v>0.0005966646527777778</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F48">
         <v>2154</v>
@@ -1871,21 +1726,18 @@
       <c r="H48">
         <v>52.76805048878428</v>
       </c>
-      <c r="I48" s="2">
-        <v>0.0004724554976851852</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F49">
         <v>2442</v>
@@ -1896,23 +1748,20 @@
       <c r="H49">
         <v>49.36745871383457</v>
       </c>
-      <c r="I49" s="2">
-        <v>0.0005725206365740741</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F50">
         <v>4088</v>
@@ -1923,17 +1772,14 @@
       <c r="H50">
         <v>49.65049536996378</v>
       </c>
-      <c r="I50" s="2">
-        <v>0.0009529575578703704</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F51">
         <v>3955</v>
@@ -1944,21 +1790,18 @@
       <c r="H51">
         <v>48.35929801716362</v>
       </c>
-      <c r="I51" s="2">
-        <v>0.0009465700462962963</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F52">
         <v>2808</v>
@@ -1969,21 +1812,18 @@
       <c r="H52">
         <v>49.25462993082829</v>
       </c>
-      <c r="I52" s="2">
-        <v>0.0006598364467592593</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F53">
         <v>2290</v>
@@ -1994,17 +1834,14 @@
       <c r="H53">
         <v>43.16258804084183</v>
       </c>
-      <c r="I53" s="2">
-        <v>0.0006140648842592592</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F54">
         <v>1740</v>
@@ -2015,21 +1852,18 @@
       <c r="H54">
         <v>45.22419504831451</v>
       </c>
-      <c r="I54" s="2">
-        <v>0.0004453122685185185</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F55">
         <v>3071</v>
@@ -2040,25 +1874,22 @@
       <c r="H55">
         <v>43.74386271896752</v>
       </c>
-      <c r="I55" s="2">
-        <v>0.0008125478472222222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56">
         <v>1497</v>
@@ -2069,21 +1900,18 @@
       <c r="H56">
         <v>53.75235031882469</v>
       </c>
-      <c r="I56" s="2">
-        <v>0.0003223373263888889</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F57">
         <v>1664</v>
@@ -2094,21 +1922,18 @@
       <c r="H57">
         <v>50.4448544975165</v>
       </c>
-      <c r="I57" s="2">
-        <v>0.0003817883796296296</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F58">
         <v>1299</v>
@@ -2119,17 +1944,14 @@
       <c r="H58">
         <v>46.91681237424967</v>
       </c>
-      <c r="I58" s="2">
-        <v>0.0003204548958333333</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59">
         <v>8111</v>
@@ -2140,21 +1962,18 @@
       <c r="H59">
         <v>50.25165509690097</v>
       </c>
-      <c r="I59" s="2">
-        <v>0.001868143738425926</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F60">
         <v>2335</v>
@@ -2165,23 +1984,20 @@
       <c r="H60">
         <v>44.4712613662878</v>
       </c>
-      <c r="I60" s="2">
-        <v>0.000607706238425926</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61">
         <v>1671</v>
@@ -2192,21 +2008,18 @@
       <c r="H61">
         <v>54.20323019463112</v>
       </c>
-      <c r="I61" s="2">
-        <v>0.0003568104282407407</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F62">
         <v>1440</v>
@@ -2217,25 +2030,22 @@
       <c r="H62">
         <v>54.65167131073039</v>
       </c>
-      <c r="I62" s="2">
-        <v>0.0003049617013888889</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F63">
         <v>1699</v>
@@ -2246,21 +2056,18 @@
       <c r="H63">
         <v>42.62714480523886</v>
       </c>
-      <c r="I63" s="2">
-        <v>0.0004613105555555556</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F64">
         <v>1609</v>
@@ -2271,21 +2078,18 @@
       <c r="H64">
         <v>43.94130632178303</v>
       </c>
-      <c r="I64" s="2">
-        <v>0.0004238081828703704</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F65">
         <v>2229</v>
@@ -2296,21 +2100,18 @@
       <c r="H65">
         <v>48.24490490299397</v>
       </c>
-      <c r="I65" s="2">
-        <v>0.0005347427083333333</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F66">
         <v>1697</v>
@@ -2321,23 +2122,20 @@
       <c r="H66">
         <v>54.59136896623828</v>
       </c>
-      <c r="I66" s="2">
-        <v>0.0003597858796296296</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F67">
         <v>1668</v>
@@ -2348,21 +2146,18 @@
       <c r="H67">
         <v>45.29266146467235</v>
       </c>
-      <c r="I67" s="2">
-        <v>0.0004262402546296296</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F68">
         <v>1616</v>
@@ -2373,21 +2168,18 @@
       <c r="H68">
         <v>45.5058239851624</v>
       </c>
-      <c r="I68" s="2">
-        <v>0.0004110178009259259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F69">
         <v>1846</v>
@@ -2398,21 +2190,18 @@
       <c r="H69">
         <v>43.26212854125188</v>
       </c>
-      <c r="I69" s="2">
-        <v>0.0004938670717592593</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F70">
         <v>1760</v>
@@ -2423,25 +2212,22 @@
       <c r="H70">
         <v>44.9563531283734</v>
       </c>
-      <c r="I70" s="2">
-        <v>0.000453114386574074</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F71">
         <v>1438</v>
@@ -2452,21 +2238,18 @@
       <c r="H71">
         <v>42.13274674861476</v>
       </c>
-      <c r="I71" s="2">
-        <v>0.0003950257175925926</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F72">
         <v>1446</v>
@@ -2477,21 +2260,18 @@
       <c r="H72">
         <v>44.16754306862344</v>
       </c>
-      <c r="I72" s="2">
-        <v>0.0003789232986111111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F73">
         <v>1525</v>
@@ -2502,21 +2282,18 @@
       <c r="H73">
         <v>45.98392528616249</v>
       </c>
-      <c r="I73" s="2">
-        <v>0.0003838398495370371</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F74">
         <v>1555</v>
@@ -2527,23 +2304,20 @@
       <c r="H74">
         <v>44.39181754032333</v>
       </c>
-      <c r="I74" s="2">
-        <v>0.0004054279861111111</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F75">
         <v>1612</v>
@@ -2554,21 +2328,18 @@
       <c r="H75">
         <v>50.90867243130535</v>
       </c>
-      <c r="I75" s="2">
-        <v>0.0003664878009259259</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F76">
         <v>1613</v>
@@ -2579,21 +2350,18 @@
       <c r="H76">
         <v>50.54455886727042</v>
       </c>
-      <c r="I76" s="2">
-        <v>0.0003693568981481481</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F77">
         <v>1632</v>
@@ -2604,21 +2372,18 @@
       <c r="H77">
         <v>44.78359603220632</v>
       </c>
-      <c r="I77" s="2">
-        <v>0.0004217814236111111</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F78">
         <v>1617</v>
@@ -2629,25 +2394,22 @@
       <c r="H78">
         <v>46.55604600796877</v>
       </c>
-      <c r="I78" s="2">
-        <v>0.0004019945717592593</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F79">
         <v>1434</v>
@@ -2658,21 +2420,18 @@
       <c r="H79">
         <v>50.31540813585413</v>
       </c>
-      <c r="I79" s="2">
-        <v>0.0003298636111111111</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F80">
         <v>1450</v>
@@ -2683,21 +2442,18 @@
       <c r="H80">
         <v>50.77945055794009</v>
       </c>
-      <c r="I80" s="2">
-        <v>0.0003304960416666666</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F81">
         <v>1505</v>
@@ -2708,21 +2464,18 @@
       <c r="H81">
         <v>53.67636944022038</v>
       </c>
-      <c r="I81" s="2">
-        <v>0.0003245186226851852</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F82">
         <v>1487</v>
@@ -2733,25 +2486,22 @@
       <c r="H82">
         <v>52.73670143175002</v>
       </c>
-      <c r="I82" s="2">
-        <v>0.0003263504861111111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F83">
         <v>2678</v>
@@ -2762,21 +2512,18 @@
       <c r="H83">
         <v>51.15854915042327</v>
       </c>
-      <c r="I83" s="2">
-        <v>0.0006058688310185185</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F84">
         <v>2642</v>
@@ -2787,21 +2534,18 @@
       <c r="H84">
         <v>50.69153557842601</v>
       </c>
-      <c r="I84" s="2">
-        <v>0.0006032309606481481</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F85">
         <v>2611</v>
@@ -2812,21 +2556,18 @@
       <c r="H85">
         <v>53.01863776702148</v>
       </c>
-      <c r="I85" s="2">
-        <v>0.0005699864930555556</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F86">
         <v>2621</v>
@@ -2837,23 +2578,20 @@
       <c r="H86">
         <v>55.31251953401408</v>
       </c>
-      <c r="I86" s="2">
-        <v>0.0005484409027777777</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F87">
         <v>1505</v>
@@ -2864,21 +2602,18 @@
       <c r="H87">
         <v>44.78316852730566</v>
       </c>
-      <c r="I87" s="2">
-        <v>0.0003889626851851851</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F88">
         <v>1512</v>
@@ -2889,21 +2624,18 @@
       <c r="H88">
         <v>44.69655297345592</v>
       </c>
-      <c r="I88" s="2">
-        <v>0.000391529074074074</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F89">
         <v>2981</v>
@@ -2914,21 +2646,18 @@
       <c r="H89">
         <v>52.3723037267541</v>
       </c>
-      <c r="I89" s="2">
-        <v>0.0006587893287037037</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F90">
         <v>2808</v>
@@ -2939,25 +2668,22 @@
       <c r="H90">
         <v>50.04585219513619</v>
       </c>
-      <c r="I90" s="2">
-        <v>0.0006494044675925926</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F91">
         <v>1278</v>
@@ -2968,21 +2694,18 @@
       <c r="H91">
         <v>60.25527302003672</v>
       </c>
-      <c r="I91" s="2">
-        <v>0.0002454833564814815</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F92">
         <v>1162</v>
@@ -2993,23 +2716,20 @@
       <c r="H92">
         <v>60.32421096632897</v>
       </c>
-      <c r="I92" s="2">
-        <v>0.0002229465393518519</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F93">
         <v>1109</v>
@@ -3020,21 +2740,18 @@
       <c r="H93">
         <v>60.33258979355374</v>
       </c>
-      <c r="I93" s="2">
-        <v>0.0002127481712962963</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F94">
         <v>1215</v>
@@ -3045,21 +2762,18 @@
       <c r="H94">
         <v>60.28341241623955</v>
       </c>
-      <c r="I94" s="2">
-        <v>0.000233273125</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F95">
         <v>1159</v>
@@ -3070,21 +2784,18 @@
       <c r="H95">
         <v>60.28903363805564</v>
       </c>
-      <c r="I95" s="2">
-        <v>0.0002225006944444445</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F96">
         <v>1194</v>
@@ -3095,25 +2806,22 @@
       <c r="H96">
         <v>60.29117912781992</v>
       </c>
-      <c r="I96" s="2">
-        <v>0.000229211712962963</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F97">
         <v>1455</v>
@@ -3124,21 +2832,18 @@
       <c r="H97">
         <v>54.94137226933356</v>
       </c>
-      <c r="I97" s="2">
-        <v>0.0003065135995370371</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F98">
         <v>1428</v>
@@ -3149,21 +2854,18 @@
       <c r="H98">
         <v>55.44917011851988</v>
       </c>
-      <c r="I98" s="2">
-        <v>0.000298070787037037</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F99">
         <v>1547</v>
@@ -3174,21 +2876,18 @@
       <c r="H99">
         <v>48.04209220174983</v>
       </c>
-      <c r="I99" s="2">
-        <v>0.0003726959375</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F100">
         <v>1548</v>
@@ -3199,23 +2898,20 @@
       <c r="H100">
         <v>49.07346570446323</v>
       </c>
-      <c r="I100" s="2">
-        <v>0.0003650988657407407</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F101">
         <v>1637</v>
@@ -3226,21 +2922,18 @@
       <c r="H101">
         <v>43.93933505103834</v>
       </c>
-      <c r="I101" s="2">
-        <v>0.0004312026851851852</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F102">
         <v>1567</v>
@@ -3251,21 +2944,18 @@
       <c r="H102">
         <v>56.13398878631331</v>
       </c>
-      <c r="I102" s="2">
-        <v>0.0003230943402777778</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F103">
         <v>1561</v>
@@ -3276,21 +2966,18 @@
       <c r="H103">
         <v>56.62011158695944</v>
       </c>
-      <c r="I103" s="2">
-        <v>0.0003190938541666667</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F104">
         <v>1624</v>
@@ -3301,25 +2988,22 @@
       <c r="H104">
         <v>57.24750808541737</v>
       </c>
-      <c r="I104" s="2">
-        <v>0.0003283338773148148</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F105">
         <v>2525</v>
@@ -3330,21 +3014,18 @@
       <c r="H105">
         <v>54.06381765835196</v>
       </c>
-      <c r="I105" s="2">
-        <v>0.0005405562962962963</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F106">
         <v>3569</v>
@@ -3355,21 +3036,18 @@
       <c r="H106">
         <v>55.63887442790875</v>
       </c>
-      <c r="I106" s="2">
-        <v>0.0007424282175925925</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F107">
         <v>2786</v>
@@ -3380,21 +3058,18 @@
       <c r="H107">
         <v>48.08498027842688</v>
       </c>
-      <c r="I107" s="2">
-        <v>0.0006705913194444444</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F108">
         <v>3111</v>
@@ -3405,23 +3080,20 @@
       <c r="H108">
         <v>46.43703248106974</v>
       </c>
-      <c r="I108" s="2">
-        <v>0.0007753928819444444</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="1"/>
       <c r="B109" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F109">
         <v>2606</v>
@@ -3432,21 +3104,18 @@
       <c r="H109">
         <v>51.51017922972792</v>
       </c>
-      <c r="I109" s="2">
-        <v>0.0005855548842592593</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F110">
         <v>2821</v>
@@ -3457,21 +3126,18 @@
       <c r="H110">
         <v>52.47464842962128</v>
       </c>
-      <c r="I110" s="2">
-        <v>0.0006222140393518518</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F111">
         <v>2760</v>
@@ -3482,21 +3148,18 @@
       <c r="H111">
         <v>52.61332982730303</v>
       </c>
-      <c r="I111" s="2">
-        <v>0.0006071549652777778</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F112">
         <v>2517</v>
@@ -3507,25 +3170,22 @@
       <c r="H112">
         <v>52.18003717407845</v>
       </c>
-      <c r="I112" s="2">
-        <v>0.0005582967361111111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F113">
         <v>1352</v>
@@ -3536,21 +3196,18 @@
       <c r="H113">
         <v>38.72691233679306</v>
       </c>
-      <c r="I113" s="2">
-        <v>0.0004040639236111112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F114">
         <v>1039</v>
@@ -3561,21 +3218,18 @@
       <c r="H114">
         <v>40.40409225401442</v>
       </c>
-      <c r="I114" s="2">
-        <v>0.0002976298263888889</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F115">
         <v>859</v>
@@ -3586,21 +3240,18 @@
       <c r="H115">
         <v>40.02647805109168</v>
       </c>
-      <c r="I115" s="2">
-        <v>0.0002483888194444444</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F116">
         <v>197</v>
@@ -3611,17 +3262,14 @@
       <c r="H116">
         <v>34.00105420527455</v>
       </c>
-      <c r="I116" s="2">
-        <v>6.705946759259259E-05</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F117">
         <v>2147</v>
@@ -3632,23 +3280,20 @@
       <c r="H117">
         <v>60.08833797308407</v>
       </c>
-      <c r="I117" s="2">
-        <v>0.0004135500810185186</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" s="1"/>
       <c r="B118" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F118">
         <v>1306</v>
@@ -3659,21 +3304,18 @@
       <c r="H118">
         <v>51.76831609400841</v>
       </c>
-      <c r="I118" s="2">
-        <v>0.0002919882638888888</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F119">
         <v>1170</v>
@@ -3684,21 +3326,18 @@
       <c r="H119">
         <v>47.58079513852783</v>
       </c>
-      <c r="I119" s="2">
-        <v>0.0002846036226851852</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F120">
         <v>1173</v>
@@ -3709,21 +3348,18 @@
       <c r="H120">
         <v>48.05961063357194</v>
       </c>
-      <c r="I120" s="2">
-        <v>0.0002824906134259259</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F121">
         <v>1238</v>
@@ -3734,25 +3370,22 @@
       <c r="H121">
         <v>43.85223694759243</v>
       </c>
-      <c r="I121" s="2">
-        <v>0.0003267496643518518</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F122">
         <v>1456</v>
@@ -3763,17 +3396,14 @@
       <c r="H122">
         <v>60.23206471339652</v>
       </c>
-      <c r="I122" s="2">
-        <v>0.0002797820717592592</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F123">
         <v>717</v>
@@ -3784,21 +3414,18 @@
       <c r="H123">
         <v>60.46067492664611</v>
       </c>
-      <c r="I123" s="2">
-        <v>0.0001372563425925926</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F124">
         <v>653</v>
@@ -3809,17 +3436,14 @@
       <c r="H124">
         <v>60.44279297908365</v>
       </c>
-      <c r="I124" s="2">
-        <v>0.000125041712962963</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F125">
         <v>731</v>
@@ -3830,17 +3454,14 @@
       <c r="H125">
         <v>60.45196735593763</v>
       </c>
-      <c r="I125" s="2">
-        <v>0.0001399565393518519</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F126">
         <v>1183</v>
@@ -3851,25 +3472,22 @@
       <c r="H126">
         <v>36.92187652394421</v>
       </c>
-      <c r="I126" s="2">
-        <v>0.0003708405671296296</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F127">
         <v>1221</v>
@@ -3880,21 +3498,18 @@
       <c r="H127">
         <v>43.52806945525566</v>
       </c>
-      <c r="I127" s="2">
-        <v>0.0003246627893518519</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F128">
         <v>1275</v>
@@ -3905,21 +3520,18 @@
       <c r="H128">
         <v>46.58122488746798</v>
       </c>
-      <c r="I128" s="2">
-        <v>0.0003168002662037037</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F129">
         <v>1442</v>
@@ -3930,21 +3542,18 @@
       <c r="H129">
         <v>52.19306613306676</v>
       </c>
-      <c r="I129" s="2">
-        <v>0.0003197707291666667</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F130">
         <v>208</v>
@@ -3955,25 +3564,22 @@
       <c r="H130">
         <v>50.56297496986884</v>
       </c>
-      <c r="I130" s="2">
-        <v>4.761206018518518E-05</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C131" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F131">
         <v>1328</v>
@@ -3984,21 +3590,18 @@
       <c r="H131">
         <v>60.25363240247975</v>
       </c>
-      <c r="I131" s="2">
-        <v>0.0002550945023148148</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F132">
         <v>1451</v>
@@ -4009,21 +3612,18 @@
       <c r="H132">
         <v>60.23019640689312</v>
       </c>
-      <c r="I132" s="2">
-        <v>0.0002788299305555555</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F133">
         <v>1610</v>
@@ -4034,21 +3634,18 @@
       <c r="H133">
         <v>60.214986201044</v>
       </c>
-      <c r="I133" s="2">
-        <v>0.0003094621527777778</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F134">
         <v>1497</v>
@@ -4059,23 +3656,20 @@
       <c r="H134">
         <v>60.24383420252938</v>
       </c>
-      <c r="I134" s="2">
-        <v>0.0002876043518518519</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" s="1"/>
       <c r="B135" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F135">
         <v>1252</v>
@@ -4086,21 +3680,18 @@
       <c r="H135">
         <v>60.27089456401301</v>
       </c>
-      <c r="I135" s="2">
-        <v>0.0002404268402777778</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F136">
         <v>1222</v>
@@ -4111,21 +3702,18 @@
       <c r="H136">
         <v>60.29797363774566</v>
       </c>
-      <c r="I136" s="2">
-        <v>0.0002345604282407407</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F137">
         <v>1287</v>
@@ -4136,21 +3724,18 @@
       <c r="H137">
         <v>60.27800101662338</v>
       </c>
-      <c r="I137" s="2">
-        <v>0.000247118900462963</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F138">
         <v>1196</v>
@@ -4160,9 +3745,6 @@
       </c>
       <c r="H138">
         <v>60.29326827172119</v>
-      </c>
-      <c r="I138" s="2">
-        <v>0.0002295876967592592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
explored vid to png
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects Outside of School\repo\Video-Processing\records\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA32F9F1-1F37-46C0-9D88-8A94244C849D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -289,8 +295,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,8 +348,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -353,13 +362,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -397,7 +414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -431,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -465,9 +483,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -640,14 +659,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -673,17 +694,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -693,17 +714,17 @@
         <v>2146</v>
       </c>
       <c r="G2">
-        <v>73.054497</v>
+        <v>73.054496999999998</v>
       </c>
       <c r="H2">
-        <v>29.37533058368741</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+        <v>29.375330583687411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
         <v>35</v>
       </c>
@@ -711,19 +732,19 @@
         <v>1138</v>
       </c>
       <c r="G3">
-        <v>38.59782</v>
+        <v>38.597819999999999</v>
       </c>
       <c r="H3">
-        <v>29.48353041700283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>29.483530417002829</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -733,17 +754,17 @@
         <v>143</v>
       </c>
       <c r="G4">
-        <v>7.703174999999999</v>
+        <v>7.7031749999999999</v>
       </c>
       <c r="H4">
         <v>18.5637740282416</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
@@ -751,15 +772,15 @@
         <v>1137</v>
       </c>
       <c r="G5">
-        <v>38.190605</v>
+        <v>38.190604999999998</v>
       </c>
       <c r="H5">
         <v>29.77172003428592</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
@@ -773,15 +794,15 @@
         <v>1790</v>
       </c>
       <c r="G6">
-        <v>36.113806</v>
+        <v>36.113805999999997</v>
       </c>
       <c r="H6">
-        <v>49.56553180797393</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+        <v>49.565531807973933</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
@@ -795,15 +816,15 @@
         <v>3872</v>
       </c>
       <c r="G7">
-        <v>72.04854</v>
+        <v>72.048540000000003</v>
       </c>
       <c r="H7">
-        <v>53.74154701816303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+        <v>53.741547018163033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -819,15 +840,15 @@
         <v>1340</v>
       </c>
       <c r="G8">
-        <v>37.059608</v>
+        <v>37.059607999999997</v>
       </c>
       <c r="H8">
-        <v>36.15796475774919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+        <v>36.157964757749191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
@@ -844,12 +865,12 @@
         <v>41.309832</v>
       </c>
       <c r="H9">
-        <v>33.84182245040358</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+        <v>33.841822450403583</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
@@ -863,15 +884,15 @@
         <v>1438</v>
       </c>
       <c r="G10">
-        <v>25.961376</v>
+        <v>25.961376000000001</v>
       </c>
       <c r="H10">
-        <v>55.38997624779211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+        <v>55.389976247792113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
@@ -885,17 +906,17 @@
         <v>1470</v>
       </c>
       <c r="G11">
-        <v>26.567759</v>
+        <v>26.567758999999999</v>
       </c>
       <c r="H11">
-        <v>55.33022186779095</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1" t="s">
+        <v>55.330221867790947</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -911,15 +932,15 @@
         <v>2582</v>
       </c>
       <c r="G12">
-        <v>48.922989</v>
+        <v>48.922989000000001</v>
       </c>
       <c r="H12">
-        <v>52.77682440866399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+        <v>52.776824408663991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
@@ -933,15 +954,15 @@
         <v>3145</v>
       </c>
       <c r="G13">
-        <v>60.784128</v>
+        <v>60.784128000000003</v>
       </c>
       <c r="H13">
         <v>51.74048067284933</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
@@ -955,15 +976,15 @@
         <v>2578</v>
       </c>
       <c r="G14">
-        <v>61.6722</v>
+        <v>61.672199999999997</v>
       </c>
       <c r="H14">
-        <v>41.80165455424</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+        <v>41.801654554240002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
@@ -977,15 +998,15 @@
         <v>2704</v>
       </c>
       <c r="G15">
-        <v>63.79880499999999</v>
+        <v>63.798804999999987</v>
       </c>
       <c r="H15">
-        <v>42.3832389964044</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+        <v>42.383238996404401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1001,15 +1022,15 @@
         <v>1188</v>
       </c>
       <c r="G16">
-        <v>26.326683</v>
+        <v>26.326682999999999</v>
       </c>
       <c r="H16">
-        <v>45.12532019320474</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+        <v>45.125320193204743</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1026,12 +1047,12 @@
         <v>29.29561</v>
       </c>
       <c r="H17">
-        <v>43.65841844563059</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+        <v>43.658418445630588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1045,15 +1066,15 @@
         <v>1406</v>
       </c>
       <c r="G18">
-        <v>25.266301</v>
+        <v>25.266300999999999</v>
       </c>
       <c r="H18">
         <v>55.64724333807311</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1067,17 +1088,17 @@
         <v>1335</v>
       </c>
       <c r="G19">
-        <v>24.610403</v>
+        <v>24.610403000000002</v>
       </c>
       <c r="H19">
-        <v>54.24535307284484</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
+        <v>54.245353072844843</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1093,15 +1114,15 @@
         <v>2495</v>
       </c>
       <c r="G20">
-        <v>56.954748</v>
+        <v>56.954748000000002</v>
       </c>
       <c r="H20">
-        <v>43.806707739274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+        <v>43.806707739274003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1115,15 +1136,15 @@
         <v>2501</v>
       </c>
       <c r="G21">
-        <v>57.296129</v>
+        <v>57.296129000000001</v>
       </c>
       <c r="H21">
-        <v>43.65041833803467</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+        <v>43.650418338034669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1140,12 +1161,12 @@
         <v>48.1372</v>
       </c>
       <c r="H22">
-        <v>55.17562301089387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+        <v>55.175623010893872</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1159,15 +1180,15 @@
         <v>2686</v>
       </c>
       <c r="G23">
-        <v>48.899545</v>
+        <v>48.899545000000003</v>
       </c>
       <c r="H23">
-        <v>54.9289364553392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
+        <v>54.928936455339198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1186,12 +1207,12 @@
         <v>27.845039</v>
       </c>
       <c r="H24">
-        <v>54.08503827198805</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+        <v>54.085038271988047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1208,12 +1229,12 @@
         <v>29.567784</v>
       </c>
       <c r="H25">
-        <v>52.08371381500893</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+        <v>52.083713815008927</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1227,15 +1248,15 @@
         <v>1519</v>
       </c>
       <c r="G26">
-        <v>29.396478</v>
+        <v>29.396477999999998</v>
       </c>
       <c r="H26">
-        <v>51.67285686400935</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+        <v>51.672856864009347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1255,11 +1276,11 @@
         <v>47.54146978146526</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1275,15 +1296,15 @@
         <v>1682</v>
       </c>
       <c r="G28">
-        <v>31.644664</v>
+        <v>31.644663999999999</v>
       </c>
       <c r="H28">
-        <v>53.15272110331144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+        <v>53.152721103311443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1297,15 +1318,15 @@
         <v>1457</v>
       </c>
       <c r="G29">
-        <v>28.055417</v>
+        <v>28.055416999999998</v>
       </c>
       <c r="H29">
-        <v>51.93292974401343</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+        <v>51.932929744013428</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1319,15 +1340,15 @@
         <v>1511</v>
       </c>
       <c r="G30">
-        <v>30.413066</v>
+        <v>30.413066000000001</v>
       </c>
       <c r="H30">
-        <v>49.68259365892278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+        <v>49.682593658922777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1341,15 +1362,15 @@
         <v>3665</v>
       </c>
       <c r="G31">
-        <v>77.43016</v>
+        <v>77.430160000000001</v>
       </c>
       <c r="H31">
-        <v>47.33297722747829</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
+        <v>47.332977227478288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1365,15 +1386,15 @@
         <v>1537</v>
       </c>
       <c r="G32">
-        <v>37.05066</v>
+        <v>37.050660000000001</v>
       </c>
       <c r="H32">
-        <v>41.48374145021978</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+        <v>41.483741450219782</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1387,15 +1408,15 @@
         <v>1563</v>
       </c>
       <c r="G33">
-        <v>36.911795</v>
+        <v>36.911794999999998</v>
       </c>
       <c r="H33">
-        <v>42.34418835496892</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+        <v>42.344188354968921</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1409,15 +1430,15 @@
         <v>1867</v>
       </c>
       <c r="G34">
-        <v>45.610873</v>
+        <v>45.610872999999998</v>
       </c>
       <c r="H34">
-        <v>40.9332222165535</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+        <v>40.933222216553503</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1431,17 +1452,17 @@
         <v>3217</v>
       </c>
       <c r="G35">
-        <v>74.95078000000001</v>
+        <v>74.950780000000009</v>
       </c>
       <c r="H35">
-        <v>42.92150128390925</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
+        <v>42.921501283909251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1457,15 +1478,15 @@
         <v>1830</v>
       </c>
       <c r="G36">
-        <v>36.819093</v>
+        <v>36.819093000000002</v>
       </c>
       <c r="H36">
-        <v>49.70247365952225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+        <v>49.702473659522248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
         <v>30</v>
       </c>
@@ -1479,15 +1500,15 @@
         <v>2103</v>
       </c>
       <c r="G37">
-        <v>39.155347</v>
+        <v>39.155346999999999</v>
       </c>
       <c r="H37">
-        <v>53.70913964828354</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+        <v>53.709139648283539</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="1" t="s">
         <v>29</v>
       </c>
@@ -1501,15 +1522,15 @@
         <v>2176</v>
       </c>
       <c r="G38">
-        <v>45.652923</v>
+        <v>45.652923000000001</v>
       </c>
       <c r="H38">
-        <v>47.66397980694467</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+        <v>47.663979806944667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1523,23 +1544,23 @@
         <v>1909</v>
       </c>
       <c r="G39">
-        <v>40.17193</v>
+        <v>40.171930000000003</v>
       </c>
       <c r="H39">
-        <v>47.5207439622642</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="1" t="s">
+        <v>47.520743962264199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -1552,14 +1573,14 @@
         <v>27.354892</v>
       </c>
       <c r="H40">
-        <v>56.15083400804507</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+        <v>56.150834008045067</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1567,17 +1588,17 @@
         <v>1413</v>
       </c>
       <c r="G41">
-        <v>27.097133</v>
+        <v>27.097132999999999</v>
       </c>
       <c r="H41">
-        <v>52.1457380749469</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+        <v>52.145738074946898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
       <c r="E42" s="1" t="s">
         <v>49</v>
       </c>
@@ -1585,15 +1606,15 @@
         <v>1420</v>
       </c>
       <c r="G42">
-        <v>27.617738</v>
+        <v>27.617737999999999</v>
       </c>
       <c r="H42">
-        <v>51.41623111929007</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+        <v>51.416231119290067</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="1" t="s">
         <v>30</v>
       </c>
@@ -1610,12 +1631,12 @@
         <v>26.896963</v>
       </c>
       <c r="H43">
-        <v>54.28122126650507</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+        <v>54.281221266505071</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="1" t="s">
         <v>29</v>
       </c>
@@ -1629,15 +1650,15 @@
         <v>1564</v>
       </c>
       <c r="G44">
-        <v>28.472678</v>
+        <v>28.472677999999998</v>
       </c>
       <c r="H44">
-        <v>54.92985240095786</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+        <v>54.929852400957863</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="1" t="s">
         <v>30</v>
       </c>
@@ -1651,17 +1672,17 @@
         <v>1713</v>
       </c>
       <c r="G45">
-        <v>31.041202</v>
+        <v>31.041201999999998</v>
       </c>
       <c r="H45">
-        <v>55.18471868454063</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="1" t="s">
+        <v>55.184718684540627</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1680,12 +1701,12 @@
         <v>42.697471</v>
       </c>
       <c r="H46">
-        <v>46.77091999195924</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+        <v>46.770919991959239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="1" t="s">
         <v>30</v>
       </c>
@@ -1699,15 +1720,15 @@
         <v>2311</v>
       </c>
       <c r="G47">
-        <v>51.55182600000001</v>
+        <v>51.551826000000013</v>
       </c>
       <c r="H47">
-        <v>44.82867396394455</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+        <v>44.828673963944553</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="1" t="s">
         <v>29</v>
       </c>
@@ -1724,12 +1745,12 @@
         <v>40.820155</v>
       </c>
       <c r="H48">
-        <v>52.76805048878428</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+        <v>52.768050488784283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="1" t="s">
         <v>30</v>
       </c>
@@ -1743,21 +1764,21 @@
         <v>2442</v>
       </c>
       <c r="G49">
-        <v>49.465783</v>
+        <v>49.465783000000002</v>
       </c>
       <c r="H49">
-        <v>49.36745871383457</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1" t="s">
+        <v>49.367458713834573</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="C50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -1767,17 +1788,17 @@
         <v>4088</v>
       </c>
       <c r="G50">
-        <v>82.335533</v>
+        <v>82.335532999999998</v>
       </c>
       <c r="H50">
-        <v>49.65049536996378</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+        <v>49.650495369963778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
       <c r="E51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1785,15 +1806,15 @@
         <v>3955</v>
       </c>
       <c r="G51">
-        <v>81.783652</v>
+        <v>81.783652000000004</v>
       </c>
       <c r="H51">
-        <v>48.35929801716362</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+        <v>48.359298017163617</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1807,19 +1828,19 @@
         <v>2808</v>
       </c>
       <c r="G52">
-        <v>57.00986900000001</v>
+        <v>57.009869000000009</v>
       </c>
       <c r="H52">
-        <v>49.25462993082829</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="1" t="s">
+        <v>49.254629930828287</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -1829,17 +1850,17 @@
         <v>2290</v>
       </c>
       <c r="G53">
-        <v>53.05520600000001</v>
+        <v>53.055206000000013</v>
       </c>
       <c r="H53">
-        <v>43.16258804084183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+        <v>43.162588040841833</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
       <c r="E54" s="1" t="s">
         <v>54</v>
       </c>
@@ -1847,15 +1868,15 @@
         <v>1740</v>
       </c>
       <c r="G54">
-        <v>38.47498</v>
+        <v>38.474980000000002</v>
       </c>
       <c r="H54">
-        <v>45.22419504831451</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+        <v>45.224195048314513</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="1" t="s">
         <v>30</v>
       </c>
@@ -1869,17 +1890,17 @@
         <v>3071</v>
       </c>
       <c r="G55">
-        <v>70.204134</v>
+        <v>70.204133999999996</v>
       </c>
       <c r="H55">
         <v>43.74386271896752</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1895,15 +1916,15 @@
         <v>1497</v>
       </c>
       <c r="G56">
-        <v>27.849945</v>
+        <v>27.849945000000002</v>
       </c>
       <c r="H56">
-        <v>53.75235031882469</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+        <v>53.752350318824689</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
       <c r="C57" s="1" t="s">
         <v>30</v>
       </c>
@@ -1917,19 +1938,19 @@
         <v>1664</v>
       </c>
       <c r="G57">
-        <v>32.986516</v>
+        <v>32.986516000000002</v>
       </c>
       <c r="H57">
-        <v>50.4448544975165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" s="1" t="s">
+        <v>50.444854497516502</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1942,14 +1963,14 @@
         <v>27.687303</v>
       </c>
       <c r="H58">
-        <v>46.91681237424967</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+        <v>46.916812374249673</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
       <c r="E59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1957,15 +1978,15 @@
         <v>8111</v>
       </c>
       <c r="G59">
-        <v>161.407619</v>
+        <v>161.40761900000001</v>
       </c>
       <c r="H59">
-        <v>50.25165509690097</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
+        <v>50.251655096900969</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="1" t="s">
         <v>30</v>
       </c>
@@ -1979,15 +2000,15 @@
         <v>2335</v>
       </c>
       <c r="G60">
-        <v>52.505819</v>
+        <v>52.505819000000002</v>
       </c>
       <c r="H60">
-        <v>44.4712613662878</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1" t="s">
+        <v>44.471261366287798</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -2003,15 +2024,15 @@
         <v>1671</v>
       </c>
       <c r="G61">
-        <v>30.828421</v>
+        <v>30.828420999999999</v>
       </c>
       <c r="H61">
-        <v>54.20323019463112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+        <v>54.203230194631118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="1" t="s">
         <v>30</v>
       </c>
@@ -2025,17 +2046,17 @@
         <v>1440</v>
       </c>
       <c r="G62">
-        <v>26.348691</v>
+        <v>26.348690999999999</v>
       </c>
       <c r="H62">
-        <v>54.65167131073039</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="1" t="s">
+        <v>54.651671310730393</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2051,15 +2072,15 @@
         <v>1699</v>
       </c>
       <c r="G63">
-        <v>39.857232</v>
+        <v>39.857232000000003</v>
       </c>
       <c r="H63">
-        <v>42.62714480523886</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+        <v>42.627144805238864</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
       <c r="C64" s="1" t="s">
         <v>30</v>
       </c>
@@ -2076,12 +2097,12 @@
         <v>36.617027</v>
       </c>
       <c r="H64">
-        <v>43.94130632178303</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+        <v>43.941306321783031</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="1" t="s">
         <v>29</v>
       </c>
@@ -2095,15 +2116,15 @@
         <v>2229</v>
       </c>
       <c r="G65">
-        <v>46.20177</v>
+        <v>46.201770000000003</v>
       </c>
       <c r="H65">
-        <v>48.24490490299397</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+        <v>48.244904902993973</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="1" t="s">
         <v>30</v>
       </c>
@@ -2120,12 +2141,12 @@
         <v>31.0855</v>
       </c>
       <c r="H66">
-        <v>54.59136896623828</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1" t="s">
+        <v>54.591368966238278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2141,15 +2162,15 @@
         <v>1668</v>
       </c>
       <c r="G67">
-        <v>36.827158</v>
+        <v>36.827157999999997</v>
       </c>
       <c r="H67">
-        <v>45.29266146467235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+        <v>45.292661464672349</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="1" t="s">
         <v>30</v>
       </c>
@@ -2163,15 +2184,15 @@
         <v>1616</v>
       </c>
       <c r="G68">
-        <v>35.511938</v>
+        <v>35.511938000000001</v>
       </c>
       <c r="H68">
-        <v>45.5058239851624</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+        <v>45.505823985162401</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="1" t="s">
         <v>29</v>
       </c>
@@ -2185,15 +2206,15 @@
         <v>1846</v>
       </c>
       <c r="G69">
-        <v>42.670115</v>
+        <v>42.670115000000003</v>
       </c>
       <c r="H69">
-        <v>43.26212854125188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+        <v>43.262128541251883</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="1" t="s">
         <v>30</v>
       </c>
@@ -2207,17 +2228,17 @@
         <v>1760</v>
       </c>
       <c r="G70">
-        <v>39.149083</v>
+        <v>39.149082999999997</v>
       </c>
       <c r="H70">
-        <v>44.9563531283734</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="1" t="s">
+        <v>44.956353128373401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2233,15 +2254,15 @@
         <v>1438</v>
       </c>
       <c r="G71">
-        <v>34.130222</v>
+        <v>34.130222000000003</v>
       </c>
       <c r="H71">
-        <v>42.13274674861476</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+        <v>42.132746748614757</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="1" t="s">
         <v>30</v>
       </c>
@@ -2255,15 +2276,15 @@
         <v>1446</v>
       </c>
       <c r="G72">
-        <v>32.73897299999999</v>
+        <v>32.738972999999987</v>
       </c>
       <c r="H72">
-        <v>44.16754306862344</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+        <v>44.167543068623438</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="1" t="s">
         <v>29</v>
       </c>
@@ -2277,15 +2298,15 @@
         <v>1525</v>
       </c>
       <c r="G73">
-        <v>33.163763</v>
+        <v>33.163763000000003</v>
       </c>
       <c r="H73">
-        <v>45.98392528616249</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+        <v>45.983925286162489</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="1" t="s">
         <v>30</v>
       </c>
@@ -2299,15 +2320,15 @@
         <v>1555</v>
       </c>
       <c r="G74">
-        <v>35.028978</v>
+        <v>35.028978000000002</v>
       </c>
       <c r="H74">
-        <v>44.39181754032333</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1" t="s">
+        <v>44.391817540323331</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2323,15 +2344,15 @@
         <v>1612</v>
       </c>
       <c r="G75">
-        <v>31.664546</v>
+        <v>31.664546000000001</v>
       </c>
       <c r="H75">
-        <v>50.90867243130535</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
+        <v>50.908672431305348</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
       <c r="C76" s="1" t="s">
         <v>30</v>
       </c>
@@ -2348,12 +2369,12 @@
         <v>31.912436</v>
       </c>
       <c r="H76">
-        <v>50.54455886727042</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+        <v>50.544558867270418</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="1" t="s">
         <v>29</v>
       </c>
@@ -2367,15 +2388,15 @@
         <v>1632</v>
       </c>
       <c r="G77">
-        <v>36.441915</v>
+        <v>36.441915000000002</v>
       </c>
       <c r="H77">
-        <v>44.78359603220632</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
+        <v>44.783596032206319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
       <c r="C78" s="1" t="s">
         <v>30</v>
       </c>
@@ -2389,17 +2410,17 @@
         <v>1617</v>
       </c>
       <c r="G78">
-        <v>34.73233099999999</v>
+        <v>34.732330999999988</v>
       </c>
       <c r="H78">
-        <v>46.55604600796877</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="1" t="s">
+        <v>46.556046007968767</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2415,15 +2436,15 @@
         <v>1434</v>
       </c>
       <c r="G79">
-        <v>28.500216</v>
+        <v>28.500216000000002</v>
       </c>
       <c r="H79">
-        <v>50.31540813585413</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
+        <v>50.315408135854128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
       <c r="C80" s="1" t="s">
         <v>30</v>
       </c>
@@ -2437,15 +2458,15 @@
         <v>1450</v>
       </c>
       <c r="G80">
-        <v>28.554858</v>
+        <v>28.554857999999999</v>
       </c>
       <c r="H80">
-        <v>50.77945055794009</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
+        <v>50.779450557940088</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
       <c r="C81" s="1" t="s">
         <v>29</v>
       </c>
@@ -2459,15 +2480,15 @@
         <v>1505</v>
       </c>
       <c r="G81">
-        <v>28.038409</v>
+        <v>28.038409000000001</v>
       </c>
       <c r="H81">
-        <v>53.67636944022038</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
+        <v>53.676369440220377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
       <c r="C82" s="1" t="s">
         <v>30</v>
       </c>
@@ -2481,17 +2502,17 @@
         <v>1487</v>
       </c>
       <c r="G82">
-        <v>28.196682</v>
+        <v>28.196681999999999</v>
       </c>
       <c r="H82">
-        <v>52.73670143175002</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="1" t="s">
+        <v>52.736701431750021</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -2507,15 +2528,15 @@
         <v>2678</v>
       </c>
       <c r="G83">
-        <v>52.347067</v>
+        <v>52.347067000000003</v>
       </c>
       <c r="H83">
-        <v>51.15854915042327</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+        <v>51.158549150423269</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
       <c r="C84" s="1" t="s">
         <v>30</v>
       </c>
@@ -2529,15 +2550,15 @@
         <v>2642</v>
       </c>
       <c r="G84">
-        <v>52.119155</v>
+        <v>52.119154999999999</v>
       </c>
       <c r="H84">
-        <v>50.69153557842601</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
+        <v>50.691535578426013</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
         <v>29</v>
       </c>
@@ -2551,15 +2572,15 @@
         <v>2611</v>
       </c>
       <c r="G85">
-        <v>49.246833</v>
+        <v>49.246833000000002</v>
       </c>
       <c r="H85">
-        <v>53.01863776702148</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
+        <v>53.018637767021481</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
       <c r="C86" s="1" t="s">
         <v>30</v>
       </c>
@@ -2573,15 +2594,15 @@
         <v>2621</v>
       </c>
       <c r="G86">
-        <v>47.38529399999999</v>
+        <v>47.385293999999988</v>
       </c>
       <c r="H86">
-        <v>55.31251953401408</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1" t="s">
+        <v>55.312519534014079</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2597,15 +2618,15 @@
         <v>1505</v>
       </c>
       <c r="G87">
-        <v>33.606376</v>
+        <v>33.606375999999997</v>
       </c>
       <c r="H87">
-        <v>44.78316852730566</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
+        <v>44.783168527305662</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
       <c r="C88" s="1" t="s">
         <v>30</v>
       </c>
@@ -2619,15 +2640,15 @@
         <v>1512</v>
       </c>
       <c r="G88">
-        <v>33.828112</v>
+        <v>33.828111999999997</v>
       </c>
       <c r="H88">
-        <v>44.69655297345592</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
+        <v>44.696552973455923</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
       <c r="C89" s="1" t="s">
         <v>29</v>
       </c>
@@ -2641,15 +2662,15 @@
         <v>2981</v>
       </c>
       <c r="G89">
-        <v>56.919398</v>
+        <v>56.919398000000001</v>
       </c>
       <c r="H89">
-        <v>52.3723037267541</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+        <v>52.372303726754097</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
       <c r="C90" s="1" t="s">
         <v>30</v>
       </c>
@@ -2663,17 +2684,17 @@
         <v>2808</v>
       </c>
       <c r="G90">
-        <v>56.108546</v>
+        <v>56.108545999999997</v>
       </c>
       <c r="H90">
-        <v>50.04585219513619</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="1" t="s">
+        <v>50.045852195136192</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2689,15 +2710,15 @@
         <v>1278</v>
       </c>
       <c r="G91">
-        <v>21.209762</v>
+        <v>21.209762000000001</v>
       </c>
       <c r="H91">
-        <v>60.25527302003672</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+        <v>60.255273020036718</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
       <c r="C92" s="1" t="s">
         <v>30</v>
       </c>
@@ -2711,15 +2732,15 @@
         <v>1162</v>
       </c>
       <c r="G92">
-        <v>19.262581</v>
+        <v>19.262581000000001</v>
       </c>
       <c r="H92">
         <v>60.32421096632897</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -2738,12 +2759,12 @@
         <v>18.381442</v>
       </c>
       <c r="H93">
-        <v>60.33258979355374</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+        <v>60.332589793553737</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
       <c r="C94" s="1" t="s">
         <v>30</v>
       </c>
@@ -2763,9 +2784,9 @@
         <v>60.28341241623955</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
       <c r="C95" s="1" t="s">
         <v>29</v>
       </c>
@@ -2779,15 +2800,15 @@
         <v>1159</v>
       </c>
       <c r="G95">
-        <v>19.22406</v>
+        <v>19.224060000000001</v>
       </c>
       <c r="H95">
-        <v>60.28903363805564</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+        <v>60.289033638055642</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
       <c r="C96" s="1" t="s">
         <v>30</v>
       </c>
@@ -2801,17 +2822,17 @@
         <v>1194</v>
       </c>
       <c r="G96">
-        <v>19.803892</v>
+        <v>19.803892000000001</v>
       </c>
       <c r="H96">
-        <v>60.29117912781992</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="1" t="s">
+        <v>60.291179127819923</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -2830,12 +2851,12 @@
         <v>26.482775</v>
       </c>
       <c r="H97">
-        <v>54.94137226933356</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
+        <v>54.941372269333563</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
       <c r="C98" s="1" t="s">
         <v>30</v>
       </c>
@@ -2849,15 +2870,15 @@
         <v>1428</v>
       </c>
       <c r="G98">
-        <v>25.753316</v>
+        <v>25.753316000000002</v>
       </c>
       <c r="H98">
-        <v>55.44917011851988</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+        <v>55.449170118519881</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
       <c r="C99" s="1" t="s">
         <v>29</v>
       </c>
@@ -2871,15 +2892,15 @@
         <v>1547</v>
       </c>
       <c r="G99">
-        <v>32.200929</v>
+        <v>32.200929000000002</v>
       </c>
       <c r="H99">
-        <v>48.04209220174983</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
+        <v>48.042092201749831</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
       <c r="C100" s="1" t="s">
         <v>30</v>
       </c>
@@ -2896,12 +2917,12 @@
         <v>31.544542</v>
       </c>
       <c r="H100">
-        <v>49.07346570446323</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1" t="s">
+        <v>49.073465704463231</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -2917,15 +2938,15 @@
         <v>1637</v>
       </c>
       <c r="G101">
-        <v>37.255912</v>
+        <v>37.255912000000002</v>
       </c>
       <c r="H101">
-        <v>43.93933505103834</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
+        <v>43.939335051038341</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
       <c r="C102" s="1" t="s">
         <v>30</v>
       </c>
@@ -2939,15 +2960,15 @@
         <v>1567</v>
       </c>
       <c r="G102">
-        <v>27.915351</v>
+        <v>27.915351000000001</v>
       </c>
       <c r="H102">
         <v>56.13398878631331</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
       <c r="C103" s="1" t="s">
         <v>29</v>
       </c>
@@ -2964,12 +2985,12 @@
         <v>27.569709</v>
       </c>
       <c r="H103">
-        <v>56.62011158695944</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
+        <v>56.620111586959439</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
       <c r="C104" s="1" t="s">
         <v>30</v>
       </c>
@@ -2983,17 +3004,17 @@
         <v>1624</v>
       </c>
       <c r="G104">
-        <v>28.368047</v>
+        <v>28.368047000000001</v>
       </c>
       <c r="H104">
-        <v>57.24750808541737</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
-      <c r="A105" s="1" t="s">
+        <v>57.247508085417373</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3009,15 +3030,15 @@
         <v>2525</v>
       </c>
       <c r="G105">
-        <v>46.704064</v>
+        <v>46.704064000000002</v>
       </c>
       <c r="H105">
-        <v>54.06381765835196</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
+        <v>54.063817658351958</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
       <c r="C106" s="1" t="s">
         <v>30</v>
       </c>
@@ -3031,15 +3052,15 @@
         <v>3569</v>
       </c>
       <c r="G106">
-        <v>64.145798</v>
+        <v>64.145797999999999</v>
       </c>
       <c r="H106">
-        <v>55.63887442790875</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
+        <v>55.638874427908753</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
       <c r="C107" s="1" t="s">
         <v>29</v>
       </c>
@@ -3056,12 +3077,12 @@
         <v>57.93909</v>
       </c>
       <c r="H107">
-        <v>48.08498027842688</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
+        <v>48.084980278426883</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
       <c r="C108" s="1" t="s">
         <v>30</v>
       </c>
@@ -3075,15 +3096,15 @@
         <v>3111</v>
       </c>
       <c r="G108">
-        <v>66.993945</v>
+        <v>66.993944999999997</v>
       </c>
       <c r="H108">
-        <v>46.43703248106974</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1" t="s">
+        <v>46.437032481069743</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -3099,15 +3120,15 @@
         <v>2606</v>
       </c>
       <c r="G109">
-        <v>50.591942</v>
+        <v>50.591942000000003</v>
       </c>
       <c r="H109">
-        <v>51.51017922972792</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+        <v>51.510179229727918</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
       <c r="C110" s="1" t="s">
         <v>30</v>
       </c>
@@ -3124,12 +3145,12 @@
         <v>53.759293</v>
       </c>
       <c r="H110">
-        <v>52.47464842962128</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
+        <v>52.474648429621283</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
       <c r="C111" s="1" t="s">
         <v>29</v>
       </c>
@@ -3143,15 +3164,15 @@
         <v>2760</v>
       </c>
       <c r="G111">
-        <v>52.458189</v>
+        <v>52.458188999999997</v>
       </c>
       <c r="H111">
-        <v>52.61332982730303</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
+        <v>52.613329827303033</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
       <c r="C112" s="1" t="s">
         <v>30</v>
       </c>
@@ -3165,17 +3186,17 @@
         <v>2517</v>
       </c>
       <c r="G112">
-        <v>48.236838</v>
+        <v>48.236837999999999</v>
       </c>
       <c r="H112">
         <v>52.18003717407845</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -3191,15 +3212,15 @@
         <v>1352</v>
       </c>
       <c r="G113">
-        <v>34.911123</v>
+        <v>34.911123000000003</v>
       </c>
       <c r="H113">
-        <v>38.72691233679306</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
+        <v>38.726912336793063</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
       <c r="C114" s="1" t="s">
         <v>30</v>
       </c>
@@ -3213,15 +3234,15 @@
         <v>1039</v>
       </c>
       <c r="G114">
-        <v>25.715217</v>
+        <v>25.715216999999999</v>
       </c>
       <c r="H114">
-        <v>40.40409225401442</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
+        <v>40.404092254014422</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
       <c r="C115" s="1" t="s">
         <v>29</v>
       </c>
@@ -3238,16 +3259,16 @@
         <v>21.460794</v>
       </c>
       <c r="H115">
-        <v>40.02647805109168</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" s="1" t="s">
+        <v>40.026478051091679</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -3257,17 +3278,17 @@
         <v>197</v>
       </c>
       <c r="G116">
-        <v>5.793938</v>
+        <v>5.7939379999999998</v>
       </c>
       <c r="H116">
-        <v>34.00105420527455</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
+        <v>34.001054205274549</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
       <c r="E117" s="1" t="s">
         <v>77</v>
       </c>
@@ -3275,15 +3296,15 @@
         <v>2147</v>
       </c>
       <c r="G117">
-        <v>35.730727</v>
+        <v>35.730727000000002</v>
       </c>
       <c r="H117">
-        <v>60.08833797308407</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1" t="s">
+        <v>60.088337973084073</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -3299,15 +3320,15 @@
         <v>1306</v>
       </c>
       <c r="G118">
-        <v>25.227786</v>
+        <v>25.227785999999998</v>
       </c>
       <c r="H118">
-        <v>51.76831609400841</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
+        <v>51.768316094008412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
         <v>30</v>
       </c>
@@ -3321,15 +3342,15 @@
         <v>1170</v>
       </c>
       <c r="G119">
-        <v>24.589753</v>
+        <v>24.589753000000002</v>
       </c>
       <c r="H119">
-        <v>47.58079513852783</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+        <v>47.580795138527833</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
         <v>29</v>
       </c>
@@ -3343,15 +3364,15 @@
         <v>1173</v>
       </c>
       <c r="G120">
-        <v>24.407189</v>
+        <v>24.407188999999999</v>
       </c>
       <c r="H120">
-        <v>48.05961063357194</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
+        <v>48.059610633571943</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
       <c r="C121" s="1" t="s">
         <v>30</v>
       </c>
@@ -3368,20 +3389,20 @@
         <v>28.231171</v>
       </c>
       <c r="H121">
-        <v>43.85223694759243</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="1" t="s">
+        <v>43.852236947592431</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -3394,14 +3415,14 @@
         <v>24.173171</v>
       </c>
       <c r="H122">
-        <v>60.23206471339652</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+        <v>60.232064713396518</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
       <c r="E123" s="1" t="s">
         <v>80</v>
       </c>
@@ -3412,16 +3433,16 @@
         <v>11.858948</v>
       </c>
       <c r="H123">
-        <v>60.46067492664611</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D124" s="1" t="s">
+        <v>60.460674926646107</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -3434,14 +3455,14 @@
         <v>10.803604</v>
       </c>
       <c r="H124">
-        <v>60.44279297908365</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
+        <v>60.442792979083649</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
       <c r="E125" s="1" t="s">
         <v>82</v>
       </c>
@@ -3452,14 +3473,14 @@
         <v>12.092245</v>
       </c>
       <c r="H125">
-        <v>60.45196735593763</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
+        <v>60.451967355937633</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
       <c r="E126" s="1" t="s">
         <v>83</v>
       </c>
@@ -3467,17 +3488,17 @@
         <v>1183</v>
       </c>
       <c r="G126">
-        <v>32.040625</v>
+        <v>32.040624999999999</v>
       </c>
       <c r="H126">
-        <v>36.92187652394421</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
-      <c r="A127" s="1" t="s">
+        <v>36.921876523944213</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -3493,15 +3514,15 @@
         <v>1221</v>
       </c>
       <c r="G127">
-        <v>28.050865</v>
+        <v>28.050865000000002</v>
       </c>
       <c r="H127">
-        <v>43.52806945525566</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
+        <v>43.528069455255661</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
       <c r="C128" s="1" t="s">
         <v>30</v>
       </c>
@@ -3515,15 +3536,15 @@
         <v>1275</v>
       </c>
       <c r="G128">
-        <v>27.371543</v>
+        <v>27.371542999999999</v>
       </c>
       <c r="H128">
-        <v>46.58122488746798</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
+        <v>46.581224887467982</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
         <v>29</v>
       </c>
@@ -3537,15 +3558,15 @@
         <v>1442</v>
       </c>
       <c r="G129">
-        <v>27.628191</v>
+        <v>27.628191000000001</v>
       </c>
       <c r="H129">
-        <v>52.19306613306676</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
+        <v>52.193066133066758</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130" s="2"/>
+      <c r="B130" s="2"/>
       <c r="C130" s="1" t="s">
         <v>30</v>
       </c>
@@ -3559,17 +3580,17 @@
         <v>208</v>
       </c>
       <c r="G130">
-        <v>4.113682</v>
+        <v>4.1136819999999998</v>
       </c>
       <c r="H130">
         <v>50.56297496986884</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -3585,15 +3606,15 @@
         <v>1328</v>
       </c>
       <c r="G131">
-        <v>22.040165</v>
+        <v>22.040164999999998</v>
       </c>
       <c r="H131">
-        <v>60.25363240247975</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
+        <v>60.253632402479752</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
         <v>30</v>
       </c>
@@ -3610,12 +3631,12 @@
         <v>24.090906</v>
       </c>
       <c r="H132">
-        <v>60.23019640689312</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
+        <v>60.230196406893121</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
       <c r="C133" s="1" t="s">
         <v>29</v>
       </c>
@@ -3632,12 +3653,12 @@
         <v>26.73753</v>
       </c>
       <c r="H133">
-        <v>60.214986201044</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
+        <v>60.214986201043999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
       <c r="C134" s="1" t="s">
         <v>30</v>
       </c>
@@ -3651,15 +3672,15 @@
         <v>1497</v>
       </c>
       <c r="G134">
-        <v>24.849016</v>
+        <v>24.849015999999999</v>
       </c>
       <c r="H134">
-        <v>60.24383420252938</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1" t="s">
+        <v>60.243834202529378</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -3678,12 +3699,12 @@
         <v>20.772879</v>
       </c>
       <c r="H135">
-        <v>60.27089456401301</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8">
-      <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
+        <v>60.270894564013012</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
       <c r="C136" s="1" t="s">
         <v>30</v>
       </c>
@@ -3697,15 +3718,15 @@
         <v>1222</v>
       </c>
       <c r="G136">
-        <v>20.266021</v>
+        <v>20.266020999999999</v>
       </c>
       <c r="H136">
-        <v>60.29797363774566</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8">
-      <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
+        <v>60.297973637745663</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
         <v>29</v>
       </c>
@@ -3722,12 +3743,12 @@
         <v>21.351073</v>
       </c>
       <c r="H137">
-        <v>60.27800101662338</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+        <v>60.278001016623378</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
         <v>30</v>
       </c>
@@ -3741,10 +3762,10 @@
         <v>1196</v>
       </c>
       <c r="G138">
-        <v>19.836377</v>
+        <v>19.836376999999999</v>
       </c>
       <c r="H138">
-        <v>60.29326827172119</v>
+        <v>60.293268271721189</v>
       </c>
     </row>
   </sheetData>
@@ -3785,21 +3806,15 @@
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B67:B70"/>
     <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B112"/>
     <mergeCell ref="B75:B78"/>
     <mergeCell ref="B79:B82"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B87:B90"/>
     <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="B113:B117"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="B127:B130"/>
-    <mergeCell ref="B131:B134"/>
     <mergeCell ref="B135:B138"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
@@ -3810,15 +3825,21 @@
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="C124:C126"/>
+    <mergeCell ref="B113:B117"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="B131:B134"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="D124:D126"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="D124:D126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
code cleanup and added xlsx with corrected fps
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects Outside of School\repo\Video-Processing\records\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA32F9F1-1F37-46C0-9D88-8A94244C849D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -295,8 +289,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,11 +342,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -362,21 +353,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -414,7 +397,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -448,7 +431,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -483,10 +465,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -659,16 +640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -694,17 +673,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -714,17 +693,17 @@
         <v>2146</v>
       </c>
       <c r="G2">
-        <v>73.054496999999998</v>
+        <v>73.054497</v>
       </c>
       <c r="H2">
-        <v>29.375330583687411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>29.37533058368741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>35</v>
       </c>
@@ -732,19 +711,19 @@
         <v>1138</v>
       </c>
       <c r="G3">
-        <v>38.597819999999999</v>
+        <v>38.59782</v>
       </c>
       <c r="H3">
-        <v>29.483530417002829</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>29.48353041700283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -754,17 +733,17 @@
         <v>143</v>
       </c>
       <c r="G4">
-        <v>7.7031749999999999</v>
+        <v>7.703174999999999</v>
       </c>
       <c r="H4">
         <v>18.5637740282416</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
@@ -772,15 +751,15 @@
         <v>1137</v>
       </c>
       <c r="G5">
-        <v>38.190604999999998</v>
+        <v>38.190605</v>
       </c>
       <c r="H5">
         <v>29.77172003428592</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
@@ -794,15 +773,15 @@
         <v>1790</v>
       </c>
       <c r="G6">
-        <v>36.113805999999997</v>
+        <v>36.113806</v>
       </c>
       <c r="H6">
-        <v>49.565531807973933</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+        <v>49.56553180797393</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
@@ -816,15 +795,15 @@
         <v>3872</v>
       </c>
       <c r="G7">
-        <v>72.048540000000003</v>
+        <v>72.04854</v>
       </c>
       <c r="H7">
-        <v>53.741547018163033</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+        <v>53.74154701816303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -840,15 +819,15 @@
         <v>1340</v>
       </c>
       <c r="G8">
-        <v>37.059607999999997</v>
+        <v>37.059608</v>
       </c>
       <c r="H8">
-        <v>36.157964757749191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+        <v>36.15796475774919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
@@ -865,12 +844,12 @@
         <v>41.309832</v>
       </c>
       <c r="H9">
-        <v>33.841822450403583</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+        <v>33.84182245040358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
@@ -884,15 +863,15 @@
         <v>1438</v>
       </c>
       <c r="G10">
-        <v>25.961376000000001</v>
+        <v>25.961376</v>
       </c>
       <c r="H10">
-        <v>55.389976247792113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+        <v>55.38997624779211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
@@ -906,17 +885,17 @@
         <v>1470</v>
       </c>
       <c r="G11">
-        <v>26.567758999999999</v>
+        <v>26.567759</v>
       </c>
       <c r="H11">
-        <v>55.330221867790947</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+        <v>55.33022186779095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -932,15 +911,15 @@
         <v>2582</v>
       </c>
       <c r="G12">
-        <v>48.922989000000001</v>
+        <v>48.922989</v>
       </c>
       <c r="H12">
-        <v>52.776824408663991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+        <v>52.77682440866399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
@@ -954,15 +933,15 @@
         <v>3145</v>
       </c>
       <c r="G13">
-        <v>60.784128000000003</v>
+        <v>60.784128</v>
       </c>
       <c r="H13">
         <v>51.74048067284933</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
@@ -976,15 +955,15 @@
         <v>2578</v>
       </c>
       <c r="G14">
-        <v>61.672199999999997</v>
+        <v>61.6722</v>
       </c>
       <c r="H14">
-        <v>41.801654554240002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+        <v>41.80165455424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
@@ -998,15 +977,15 @@
         <v>2704</v>
       </c>
       <c r="G15">
-        <v>63.798804999999987</v>
+        <v>63.79880499999999</v>
       </c>
       <c r="H15">
-        <v>42.383238996404401</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
+        <v>42.3832389964044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1022,15 +1001,15 @@
         <v>1188</v>
       </c>
       <c r="G16">
-        <v>26.326682999999999</v>
+        <v>26.326683</v>
       </c>
       <c r="H16">
-        <v>45.125320193204743</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+        <v>45.12532019320474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1047,12 +1026,12 @@
         <v>29.29561</v>
       </c>
       <c r="H17">
-        <v>43.658418445630588</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+        <v>43.65841844563059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1066,15 +1045,15 @@
         <v>1406</v>
       </c>
       <c r="G18">
-        <v>25.266300999999999</v>
+        <v>25.266301</v>
       </c>
       <c r="H18">
         <v>55.64724333807311</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1088,17 +1067,17 @@
         <v>1335</v>
       </c>
       <c r="G19">
-        <v>24.610403000000002</v>
+        <v>24.610403</v>
       </c>
       <c r="H19">
-        <v>54.245353072844843</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+        <v>54.24535307284484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1114,15 +1093,15 @@
         <v>2495</v>
       </c>
       <c r="G20">
-        <v>56.954748000000002</v>
+        <v>56.954748</v>
       </c>
       <c r="H20">
-        <v>43.806707739274003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+        <v>43.806707739274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1136,15 +1115,15 @@
         <v>2501</v>
       </c>
       <c r="G21">
-        <v>57.296129000000001</v>
+        <v>57.296129</v>
       </c>
       <c r="H21">
-        <v>43.650418338034669</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+        <v>43.65041833803467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1161,12 +1140,12 @@
         <v>48.1372</v>
       </c>
       <c r="H22">
-        <v>55.175623010893872</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+        <v>55.17562301089387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1180,15 +1159,15 @@
         <v>2686</v>
       </c>
       <c r="G23">
-        <v>48.899545000000003</v>
+        <v>48.899545</v>
       </c>
       <c r="H23">
-        <v>54.928936455339198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
+        <v>54.9289364553392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1207,12 +1186,12 @@
         <v>27.845039</v>
       </c>
       <c r="H24">
-        <v>54.085038271988047</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+        <v>54.08503827198805</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1229,12 +1208,12 @@
         <v>29.567784</v>
       </c>
       <c r="H25">
-        <v>52.083713815008927</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+        <v>52.08371381500893</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1248,15 +1227,15 @@
         <v>1519</v>
       </c>
       <c r="G26">
-        <v>29.396477999999998</v>
+        <v>29.396478</v>
       </c>
       <c r="H26">
-        <v>51.672856864009347</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+        <v>51.67285686400935</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1276,11 +1255,11 @@
         <v>47.54146978146526</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1296,15 +1275,15 @@
         <v>1682</v>
       </c>
       <c r="G28">
-        <v>31.644663999999999</v>
+        <v>31.644664</v>
       </c>
       <c r="H28">
-        <v>53.152721103311443</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+        <v>53.15272110331144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1318,15 +1297,15 @@
         <v>1457</v>
       </c>
       <c r="G29">
-        <v>28.055416999999998</v>
+        <v>28.055417</v>
       </c>
       <c r="H29">
-        <v>51.932929744013428</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+        <v>51.93292974401343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1340,15 +1319,15 @@
         <v>1511</v>
       </c>
       <c r="G30">
-        <v>30.413066000000001</v>
+        <v>30.413066</v>
       </c>
       <c r="H30">
-        <v>49.682593658922777</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+        <v>49.68259365892278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1362,15 +1341,15 @@
         <v>3665</v>
       </c>
       <c r="G31">
-        <v>77.430160000000001</v>
+        <v>77.43016</v>
       </c>
       <c r="H31">
-        <v>47.332977227478288</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2" t="s">
+        <v>47.33297722747829</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1386,15 +1365,15 @@
         <v>1537</v>
       </c>
       <c r="G32">
-        <v>37.050660000000001</v>
+        <v>37.05066</v>
       </c>
       <c r="H32">
-        <v>41.483741450219782</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+        <v>41.48374145021978</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1408,15 +1387,15 @@
         <v>1563</v>
       </c>
       <c r="G33">
-        <v>36.911794999999998</v>
+        <v>36.911795</v>
       </c>
       <c r="H33">
-        <v>42.344188354968921</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+        <v>42.34418835496892</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1430,15 +1409,15 @@
         <v>1867</v>
       </c>
       <c r="G34">
-        <v>45.610872999999998</v>
+        <v>45.610873</v>
       </c>
       <c r="H34">
-        <v>40.933222216553503</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+        <v>40.9332222165535</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1452,17 +1431,17 @@
         <v>3217</v>
       </c>
       <c r="G35">
-        <v>74.950780000000009</v>
+        <v>74.95078000000001</v>
       </c>
       <c r="H35">
-        <v>42.921501283909251</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+        <v>42.92150128390925</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1478,15 +1457,15 @@
         <v>1830</v>
       </c>
       <c r="G36">
-        <v>36.819093000000002</v>
+        <v>36.819093</v>
       </c>
       <c r="H36">
-        <v>49.702473659522248</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+        <v>49.70247365952225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>30</v>
       </c>
@@ -1500,15 +1479,15 @@
         <v>2103</v>
       </c>
       <c r="G37">
-        <v>39.155346999999999</v>
+        <v>39.155347</v>
       </c>
       <c r="H37">
-        <v>53.709139648283539</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+        <v>53.70913964828354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
         <v>29</v>
       </c>
@@ -1522,15 +1501,15 @@
         <v>2176</v>
       </c>
       <c r="G38">
-        <v>45.652923000000001</v>
+        <v>45.652923</v>
       </c>
       <c r="H38">
-        <v>47.663979806944667</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+        <v>47.66397980694467</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1544,23 +1523,23 @@
         <v>1909</v>
       </c>
       <c r="G39">
-        <v>40.171930000000003</v>
+        <v>40.17193</v>
       </c>
       <c r="H39">
-        <v>47.520743962264199</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+        <v>47.5207439622642</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -1573,14 +1552,14 @@
         <v>27.354892</v>
       </c>
       <c r="H40">
-        <v>56.150834008045067</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+        <v>56.15083400804507</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1588,17 +1567,17 @@
         <v>1413</v>
       </c>
       <c r="G41">
-        <v>27.097132999999999</v>
+        <v>27.097133</v>
       </c>
       <c r="H41">
-        <v>52.145738074946898</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+        <v>52.1457380749469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
         <v>49</v>
       </c>
@@ -1606,15 +1585,15 @@
         <v>1420</v>
       </c>
       <c r="G42">
-        <v>27.617737999999999</v>
+        <v>27.617738</v>
       </c>
       <c r="H42">
-        <v>51.416231119290067</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+        <v>51.41623111929007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>30</v>
       </c>
@@ -1631,12 +1610,12 @@
         <v>26.896963</v>
       </c>
       <c r="H43">
-        <v>54.281221266505071</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+        <v>54.28122126650507</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
         <v>29</v>
       </c>
@@ -1650,15 +1629,15 @@
         <v>1564</v>
       </c>
       <c r="G44">
-        <v>28.472677999999998</v>
+        <v>28.472678</v>
       </c>
       <c r="H44">
-        <v>54.929852400957863</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+        <v>54.92985240095786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
         <v>30</v>
       </c>
@@ -1672,17 +1651,17 @@
         <v>1713</v>
       </c>
       <c r="G45">
-        <v>31.041201999999998</v>
+        <v>31.041202</v>
       </c>
       <c r="H45">
-        <v>55.184718684540627</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+        <v>55.18471868454063</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1701,12 +1680,12 @@
         <v>42.697471</v>
       </c>
       <c r="H46">
-        <v>46.770919991959239</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
+        <v>46.77091999195924</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
         <v>30</v>
       </c>
@@ -1720,15 +1699,15 @@
         <v>2311</v>
       </c>
       <c r="G47">
-        <v>51.551826000000013</v>
+        <v>51.55182600000001</v>
       </c>
       <c r="H47">
-        <v>44.828673963944553</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+        <v>44.82867396394455</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
         <v>29</v>
       </c>
@@ -1745,12 +1724,12 @@
         <v>40.820155</v>
       </c>
       <c r="H48">
-        <v>52.768050488784283</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+        <v>52.76805048878428</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>30</v>
       </c>
@@ -1764,21 +1743,21 @@
         <v>2442</v>
       </c>
       <c r="G49">
-        <v>49.465783000000002</v>
+        <v>49.465783</v>
       </c>
       <c r="H49">
-        <v>49.367458713834573</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2" t="s">
+        <v>49.36745871383457</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -1788,17 +1767,17 @@
         <v>4088</v>
       </c>
       <c r="G50">
-        <v>82.335532999999998</v>
+        <v>82.335533</v>
       </c>
       <c r="H50">
-        <v>49.650495369963778</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+        <v>49.65049536996378</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1806,15 +1785,15 @@
         <v>3955</v>
       </c>
       <c r="G51">
-        <v>81.783652000000004</v>
+        <v>81.783652</v>
       </c>
       <c r="H51">
-        <v>48.359298017163617</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+        <v>48.35929801716362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1828,19 +1807,19 @@
         <v>2808</v>
       </c>
       <c r="G52">
-        <v>57.009869000000009</v>
+        <v>57.00986900000001</v>
       </c>
       <c r="H52">
-        <v>49.254629930828287</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="2" t="s">
+        <v>49.25462993082829</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -1850,17 +1829,17 @@
         <v>2290</v>
       </c>
       <c r="G53">
-        <v>53.055206000000013</v>
+        <v>53.05520600000001</v>
       </c>
       <c r="H53">
-        <v>43.162588040841833</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+        <v>43.16258804084183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
         <v>54</v>
       </c>
@@ -1868,15 +1847,15 @@
         <v>1740</v>
       </c>
       <c r="G54">
-        <v>38.474980000000002</v>
+        <v>38.47498</v>
       </c>
       <c r="H54">
-        <v>45.224195048314513</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
+        <v>45.22419504831451</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>30</v>
       </c>
@@ -1890,17 +1869,17 @@
         <v>3071</v>
       </c>
       <c r="G55">
-        <v>70.204133999999996</v>
+        <v>70.204134</v>
       </c>
       <c r="H55">
         <v>43.74386271896752</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:8">
+      <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1916,15 +1895,15 @@
         <v>1497</v>
       </c>
       <c r="G56">
-        <v>27.849945000000002</v>
+        <v>27.849945</v>
       </c>
       <c r="H56">
-        <v>53.752350318824689</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+        <v>53.75235031882469</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>30</v>
       </c>
@@ -1938,19 +1917,19 @@
         <v>1664</v>
       </c>
       <c r="G57">
-        <v>32.986516000000002</v>
+        <v>32.986516</v>
       </c>
       <c r="H57">
-        <v>50.444854497516502</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" s="2" t="s">
+        <v>50.4448544975165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1963,14 +1942,14 @@
         <v>27.687303</v>
       </c>
       <c r="H58">
-        <v>46.916812374249673</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+        <v>46.91681237424967</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1978,15 +1957,15 @@
         <v>8111</v>
       </c>
       <c r="G59">
-        <v>161.40761900000001</v>
+        <v>161.407619</v>
       </c>
       <c r="H59">
-        <v>50.251655096900969</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+        <v>50.25165509690097</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>30</v>
       </c>
@@ -2000,15 +1979,15 @@
         <v>2335</v>
       </c>
       <c r="G60">
-        <v>52.505819000000002</v>
+        <v>52.505819</v>
       </c>
       <c r="H60">
-        <v>44.471261366287798</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2" t="s">
+        <v>44.4712613662878</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -2024,15 +2003,15 @@
         <v>1671</v>
       </c>
       <c r="G61">
-        <v>30.828420999999999</v>
+        <v>30.828421</v>
       </c>
       <c r="H61">
-        <v>54.203230194631118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+        <v>54.20323019463112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
         <v>30</v>
       </c>
@@ -2046,17 +2025,17 @@
         <v>1440</v>
       </c>
       <c r="G62">
-        <v>26.348690999999999</v>
+        <v>26.348691</v>
       </c>
       <c r="H62">
-        <v>54.651671310730393</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+        <v>54.65167131073039</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2072,15 +2051,15 @@
         <v>1699</v>
       </c>
       <c r="G63">
-        <v>39.857232000000003</v>
+        <v>39.857232</v>
       </c>
       <c r="H63">
-        <v>42.627144805238864</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
+        <v>42.62714480523886</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
         <v>30</v>
       </c>
@@ -2097,12 +2076,12 @@
         <v>36.617027</v>
       </c>
       <c r="H64">
-        <v>43.941306321783031</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
+        <v>43.94130632178303</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
         <v>29</v>
       </c>
@@ -2116,15 +2095,15 @@
         <v>2229</v>
       </c>
       <c r="G65">
-        <v>46.201770000000003</v>
+        <v>46.20177</v>
       </c>
       <c r="H65">
-        <v>48.244904902993973</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+        <v>48.24490490299397</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
         <v>30</v>
       </c>
@@ -2141,12 +2120,12 @@
         <v>31.0855</v>
       </c>
       <c r="H66">
-        <v>54.591368966238278</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2" t="s">
+        <v>54.59136896623828</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2162,15 +2141,15 @@
         <v>1668</v>
       </c>
       <c r="G67">
-        <v>36.827157999999997</v>
+        <v>36.827158</v>
       </c>
       <c r="H67">
-        <v>45.292661464672349</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
+        <v>45.29266146467235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
         <v>30</v>
       </c>
@@ -2184,15 +2163,15 @@
         <v>1616</v>
       </c>
       <c r="G68">
-        <v>35.511938000000001</v>
+        <v>35.511938</v>
       </c>
       <c r="H68">
-        <v>45.505823985162401</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
+        <v>45.5058239851624</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
         <v>29</v>
       </c>
@@ -2206,15 +2185,15 @@
         <v>1846</v>
       </c>
       <c r="G69">
-        <v>42.670115000000003</v>
+        <v>42.670115</v>
       </c>
       <c r="H69">
-        <v>43.262128541251883</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
+        <v>43.26212854125188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
         <v>30</v>
       </c>
@@ -2228,17 +2207,17 @@
         <v>1760</v>
       </c>
       <c r="G70">
-        <v>39.149082999999997</v>
+        <v>39.149083</v>
       </c>
       <c r="H70">
-        <v>44.956353128373401</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+        <v>44.9563531283734</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2254,15 +2233,15 @@
         <v>1438</v>
       </c>
       <c r="G71">
-        <v>34.130222000000003</v>
+        <v>34.130222</v>
       </c>
       <c r="H71">
-        <v>42.132746748614757</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
+        <v>42.13274674861476</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
         <v>30</v>
       </c>
@@ -2276,15 +2255,15 @@
         <v>1446</v>
       </c>
       <c r="G72">
-        <v>32.738972999999987</v>
+        <v>32.73897299999999</v>
       </c>
       <c r="H72">
-        <v>44.167543068623438</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
+        <v>44.16754306862344</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
         <v>29</v>
       </c>
@@ -2298,15 +2277,15 @@
         <v>1525</v>
       </c>
       <c r="G73">
-        <v>33.163763000000003</v>
+        <v>33.163763</v>
       </c>
       <c r="H73">
-        <v>45.983925286162489</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
+        <v>45.98392528616249</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
         <v>30</v>
       </c>
@@ -2320,15 +2299,15 @@
         <v>1555</v>
       </c>
       <c r="G74">
-        <v>35.028978000000002</v>
+        <v>35.028978</v>
       </c>
       <c r="H74">
-        <v>44.391817540323331</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2" t="s">
+        <v>44.39181754032333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2344,15 +2323,15 @@
         <v>1612</v>
       </c>
       <c r="G75">
-        <v>31.664546000000001</v>
+        <v>31.664546</v>
       </c>
       <c r="H75">
-        <v>50.908672431305348</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
+        <v>50.90867243130535</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
         <v>30</v>
       </c>
@@ -2369,12 +2348,12 @@
         <v>31.912436</v>
       </c>
       <c r="H76">
-        <v>50.544558867270418</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
+        <v>50.54455886727042</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
         <v>29</v>
       </c>
@@ -2388,15 +2367,15 @@
         <v>1632</v>
       </c>
       <c r="G77">
-        <v>36.441915000000002</v>
+        <v>36.441915</v>
       </c>
       <c r="H77">
-        <v>44.783596032206319</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
+        <v>44.78359603220632</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
         <v>30</v>
       </c>
@@ -2410,17 +2389,17 @@
         <v>1617</v>
       </c>
       <c r="G78">
-        <v>34.732330999999988</v>
+        <v>34.73233099999999</v>
       </c>
       <c r="H78">
-        <v>46.556046007968767</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+        <v>46.55604600796877</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2436,15 +2415,15 @@
         <v>1434</v>
       </c>
       <c r="G79">
-        <v>28.500216000000002</v>
+        <v>28.500216</v>
       </c>
       <c r="H79">
-        <v>50.315408135854128</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
+        <v>50.31540813585413</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
         <v>30</v>
       </c>
@@ -2458,15 +2437,15 @@
         <v>1450</v>
       </c>
       <c r="G80">
-        <v>28.554857999999999</v>
+        <v>28.554858</v>
       </c>
       <c r="H80">
-        <v>50.779450557940088</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
+        <v>50.77945055794009</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
         <v>29</v>
       </c>
@@ -2480,15 +2459,15 @@
         <v>1505</v>
       </c>
       <c r="G81">
-        <v>28.038409000000001</v>
+        <v>28.038409</v>
       </c>
       <c r="H81">
-        <v>53.676369440220377</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
+        <v>53.67636944022038</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
         <v>30</v>
       </c>
@@ -2502,17 +2481,17 @@
         <v>1487</v>
       </c>
       <c r="G82">
-        <v>28.196681999999999</v>
+        <v>28.196682</v>
       </c>
       <c r="H82">
-        <v>52.736701431750021</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
+        <v>52.73670143175002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -2528,15 +2507,15 @@
         <v>2678</v>
       </c>
       <c r="G83">
-        <v>52.347067000000003</v>
+        <v>52.347067</v>
       </c>
       <c r="H83">
-        <v>51.158549150423269</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
+        <v>51.15854915042327</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
         <v>30</v>
       </c>
@@ -2550,15 +2529,15 @@
         <v>2642</v>
       </c>
       <c r="G84">
-        <v>52.119154999999999</v>
+        <v>52.119155</v>
       </c>
       <c r="H84">
-        <v>50.691535578426013</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
+        <v>50.69153557842601</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
         <v>29</v>
       </c>
@@ -2572,15 +2551,15 @@
         <v>2611</v>
       </c>
       <c r="G85">
-        <v>49.246833000000002</v>
+        <v>49.246833</v>
       </c>
       <c r="H85">
-        <v>53.018637767021481</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
+        <v>53.01863776702148</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
         <v>30</v>
       </c>
@@ -2594,15 +2573,15 @@
         <v>2621</v>
       </c>
       <c r="G86">
-        <v>47.385293999999988</v>
+        <v>47.38529399999999</v>
       </c>
       <c r="H86">
-        <v>55.312519534014079</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2" t="s">
+        <v>55.31251953401408</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2618,15 +2597,15 @@
         <v>1505</v>
       </c>
       <c r="G87">
-        <v>33.606375999999997</v>
+        <v>33.606376</v>
       </c>
       <c r="H87">
-        <v>44.783168527305662</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
+        <v>44.78316852730566</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
         <v>30</v>
       </c>
@@ -2640,15 +2619,15 @@
         <v>1512</v>
       </c>
       <c r="G88">
-        <v>33.828111999999997</v>
+        <v>33.828112</v>
       </c>
       <c r="H88">
-        <v>44.696552973455923</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
+        <v>44.69655297345592</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
         <v>29</v>
       </c>
@@ -2662,15 +2641,15 @@
         <v>2981</v>
       </c>
       <c r="G89">
-        <v>56.919398000000001</v>
+        <v>56.919398</v>
       </c>
       <c r="H89">
-        <v>52.372303726754097</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
+        <v>52.3723037267541</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
         <v>30</v>
       </c>
@@ -2684,17 +2663,17 @@
         <v>2808</v>
       </c>
       <c r="G90">
-        <v>56.108545999999997</v>
+        <v>56.108546</v>
       </c>
       <c r="H90">
-        <v>50.045852195136192</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A91" s="2" t="s">
+        <v>50.04585219513619</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2710,15 +2689,15 @@
         <v>1278</v>
       </c>
       <c r="G91">
-        <v>21.209762000000001</v>
+        <v>21.209762</v>
       </c>
       <c r="H91">
-        <v>60.255273020036718</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
+        <v>60.25527302003672</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
         <v>30</v>
       </c>
@@ -2732,15 +2711,15 @@
         <v>1162</v>
       </c>
       <c r="G92">
-        <v>19.262581000000001</v>
+        <v>19.262581</v>
       </c>
       <c r="H92">
         <v>60.32421096632897</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2" t="s">
+    <row r="93" spans="1:8">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -2759,12 +2738,12 @@
         <v>18.381442</v>
       </c>
       <c r="H93">
-        <v>60.332589793553737</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
+        <v>60.33258979355374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
         <v>30</v>
       </c>
@@ -2784,9 +2763,9 @@
         <v>60.28341241623955</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
+    <row r="95" spans="1:8">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
         <v>29</v>
       </c>
@@ -2800,15 +2779,15 @@
         <v>1159</v>
       </c>
       <c r="G95">
-        <v>19.224060000000001</v>
+        <v>19.22406</v>
       </c>
       <c r="H95">
-        <v>60.289033638055642</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
+        <v>60.28903363805564</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
         <v>30</v>
       </c>
@@ -2822,17 +2801,17 @@
         <v>1194</v>
       </c>
       <c r="G96">
-        <v>19.803892000000001</v>
+        <v>19.803892</v>
       </c>
       <c r="H96">
-        <v>60.291179127819923</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="2" t="s">
+        <v>60.29117912781992</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -2851,12 +2830,12 @@
         <v>26.482775</v>
       </c>
       <c r="H97">
-        <v>54.941372269333563</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
+        <v>54.94137226933356</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
         <v>30</v>
       </c>
@@ -2870,15 +2849,15 @@
         <v>1428</v>
       </c>
       <c r="G98">
-        <v>25.753316000000002</v>
+        <v>25.753316</v>
       </c>
       <c r="H98">
-        <v>55.449170118519881</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
+        <v>55.44917011851988</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
         <v>29</v>
       </c>
@@ -2892,15 +2871,15 @@
         <v>1547</v>
       </c>
       <c r="G99">
-        <v>32.200929000000002</v>
+        <v>32.200929</v>
       </c>
       <c r="H99">
-        <v>48.042092201749831</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
+        <v>48.04209220174983</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
         <v>30</v>
       </c>
@@ -2917,12 +2896,12 @@
         <v>31.544542</v>
       </c>
       <c r="H100">
-        <v>49.073465704463231</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2" t="s">
+        <v>49.07346570446323</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -2938,15 +2917,15 @@
         <v>1637</v>
       </c>
       <c r="G101">
-        <v>37.255912000000002</v>
+        <v>37.255912</v>
       </c>
       <c r="H101">
-        <v>43.939335051038341</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
+        <v>43.93933505103834</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
         <v>30</v>
       </c>
@@ -2960,15 +2939,15 @@
         <v>1567</v>
       </c>
       <c r="G102">
-        <v>27.915351000000001</v>
+        <v>27.915351</v>
       </c>
       <c r="H102">
         <v>56.13398878631331</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
+    <row r="103" spans="1:8">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
         <v>29</v>
       </c>
@@ -2985,12 +2964,12 @@
         <v>27.569709</v>
       </c>
       <c r="H103">
-        <v>56.620111586959439</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
+        <v>56.62011158695944</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
       <c r="C104" s="1" t="s">
         <v>30</v>
       </c>
@@ -3004,17 +2983,17 @@
         <v>1624</v>
       </c>
       <c r="G104">
-        <v>28.368047000000001</v>
+        <v>28.368047</v>
       </c>
       <c r="H104">
-        <v>57.247508085417373</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A105" s="2" t="s">
+        <v>57.24750808541737</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3030,15 +3009,15 @@
         <v>2525</v>
       </c>
       <c r="G105">
-        <v>46.704064000000002</v>
+        <v>46.704064</v>
       </c>
       <c r="H105">
-        <v>54.063817658351958</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
+        <v>54.06381765835196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
       <c r="C106" s="1" t="s">
         <v>30</v>
       </c>
@@ -3052,15 +3031,15 @@
         <v>3569</v>
       </c>
       <c r="G106">
-        <v>64.145797999999999</v>
+        <v>64.145798</v>
       </c>
       <c r="H106">
-        <v>55.638874427908753</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
+        <v>55.63887442790875</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
       <c r="C107" s="1" t="s">
         <v>29</v>
       </c>
@@ -3077,12 +3056,12 @@
         <v>57.93909</v>
       </c>
       <c r="H107">
-        <v>48.084980278426883</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
+        <v>48.08498027842688</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
         <v>30</v>
       </c>
@@ -3096,15 +3075,15 @@
         <v>3111</v>
       </c>
       <c r="G108">
-        <v>66.993944999999997</v>
+        <v>66.993945</v>
       </c>
       <c r="H108">
-        <v>46.437032481069743</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2" t="s">
+        <v>46.43703248106974</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -3120,15 +3099,15 @@
         <v>2606</v>
       </c>
       <c r="G109">
-        <v>50.591942000000003</v>
+        <v>50.591942</v>
       </c>
       <c r="H109">
-        <v>51.510179229727918</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
+        <v>51.51017922972792</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
         <v>30</v>
       </c>
@@ -3145,12 +3124,12 @@
         <v>53.759293</v>
       </c>
       <c r="H110">
-        <v>52.474648429621283</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
+        <v>52.47464842962128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
         <v>29</v>
       </c>
@@ -3164,15 +3143,15 @@
         <v>2760</v>
       </c>
       <c r="G111">
-        <v>52.458188999999997</v>
+        <v>52.458189</v>
       </c>
       <c r="H111">
-        <v>52.613329827303033</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
+        <v>52.61332982730303</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
         <v>30</v>
       </c>
@@ -3186,17 +3165,17 @@
         <v>2517</v>
       </c>
       <c r="G112">
-        <v>48.236837999999999</v>
+        <v>48.236838</v>
       </c>
       <c r="H112">
         <v>52.18003717407845</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:8">
+      <c r="A113" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -3212,15 +3191,15 @@
         <v>1352</v>
       </c>
       <c r="G113">
-        <v>34.911123000000003</v>
+        <v>34.911123</v>
       </c>
       <c r="H113">
-        <v>38.726912336793063</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A114" s="2"/>
-      <c r="B114" s="2"/>
+        <v>38.72691233679306</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
         <v>30</v>
       </c>
@@ -3234,15 +3213,15 @@
         <v>1039</v>
       </c>
       <c r="G114">
-        <v>25.715216999999999</v>
+        <v>25.715217</v>
       </c>
       <c r="H114">
-        <v>40.404092254014422</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
+        <v>40.40409225401442</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
         <v>29</v>
       </c>
@@ -3259,16 +3238,16 @@
         <v>21.460794</v>
       </c>
       <c r="H115">
-        <v>40.026478051091679</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" s="2" t="s">
+        <v>40.02647805109168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -3278,17 +3257,17 @@
         <v>197</v>
       </c>
       <c r="G116">
-        <v>5.7939379999999998</v>
+        <v>5.793938</v>
       </c>
       <c r="H116">
-        <v>34.001054205274549</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
+        <v>34.00105420527455</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
       <c r="E117" s="1" t="s">
         <v>77</v>
       </c>
@@ -3296,15 +3275,15 @@
         <v>2147</v>
       </c>
       <c r="G117">
-        <v>35.730727000000002</v>
+        <v>35.730727</v>
       </c>
       <c r="H117">
-        <v>60.088337973084073</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2" t="s">
+        <v>60.08833797308407</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -3320,15 +3299,15 @@
         <v>1306</v>
       </c>
       <c r="G118">
-        <v>25.227785999999998</v>
+        <v>25.227786</v>
       </c>
       <c r="H118">
-        <v>51.768316094008412</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
+        <v>51.76831609400841</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
       <c r="C119" s="1" t="s">
         <v>30</v>
       </c>
@@ -3342,15 +3321,15 @@
         <v>1170</v>
       </c>
       <c r="G119">
-        <v>24.589753000000002</v>
+        <v>24.589753</v>
       </c>
       <c r="H119">
-        <v>47.580795138527833</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
+        <v>47.58079513852783</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
         <v>29</v>
       </c>
@@ -3364,15 +3343,15 @@
         <v>1173</v>
       </c>
       <c r="G120">
-        <v>24.407188999999999</v>
+        <v>24.407189</v>
       </c>
       <c r="H120">
-        <v>48.059610633571943</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
+        <v>48.05961063357194</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
         <v>30</v>
       </c>
@@ -3389,20 +3368,20 @@
         <v>28.231171</v>
       </c>
       <c r="H121">
-        <v>43.852236947592431</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A122" s="2" t="s">
+        <v>43.85223694759243</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -3415,14 +3394,14 @@
         <v>24.173171</v>
       </c>
       <c r="H122">
-        <v>60.232064713396518</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
+        <v>60.23206471339652</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
       <c r="E123" s="1" t="s">
         <v>80</v>
       </c>
@@ -3433,16 +3412,16 @@
         <v>11.858948</v>
       </c>
       <c r="H123">
-        <v>60.460674926646107</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D124" s="2" t="s">
+        <v>60.46067492664611</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -3455,14 +3434,14 @@
         <v>10.803604</v>
       </c>
       <c r="H124">
-        <v>60.442792979083649</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
+        <v>60.44279297908365</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
       <c r="E125" s="1" t="s">
         <v>82</v>
       </c>
@@ -3473,14 +3452,14 @@
         <v>12.092245</v>
       </c>
       <c r="H125">
-        <v>60.451967355937633</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
+        <v>60.45196735593763</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
       <c r="E126" s="1" t="s">
         <v>83</v>
       </c>
@@ -3488,17 +3467,17 @@
         <v>1183</v>
       </c>
       <c r="G126">
-        <v>32.040624999999999</v>
+        <v>32.040625</v>
       </c>
       <c r="H126">
-        <v>36.921876523944213</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A127" s="2" t="s">
+        <v>36.92187652394421</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -3514,15 +3493,15 @@
         <v>1221</v>
       </c>
       <c r="G127">
-        <v>28.050865000000002</v>
+        <v>28.050865</v>
       </c>
       <c r="H127">
-        <v>43.528069455255661</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
+        <v>43.52806945525566</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
         <v>30</v>
       </c>
@@ -3536,15 +3515,15 @@
         <v>1275</v>
       </c>
       <c r="G128">
-        <v>27.371542999999999</v>
+        <v>27.371543</v>
       </c>
       <c r="H128">
-        <v>46.581224887467982</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
+        <v>46.58122488746798</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
         <v>29</v>
       </c>
@@ -3558,15 +3537,15 @@
         <v>1442</v>
       </c>
       <c r="G129">
-        <v>27.628191000000001</v>
+        <v>27.628191</v>
       </c>
       <c r="H129">
-        <v>52.193066133066758</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
+        <v>52.19306613306676</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
         <v>30</v>
       </c>
@@ -3580,17 +3559,17 @@
         <v>208</v>
       </c>
       <c r="G130">
-        <v>4.1136819999999998</v>
+        <v>4.113682</v>
       </c>
       <c r="H130">
         <v>50.56297496986884</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
+    <row r="131" spans="1:8">
+      <c r="A131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -3606,15 +3585,15 @@
         <v>1328</v>
       </c>
       <c r="G131">
-        <v>22.040164999999998</v>
+        <v>22.040165</v>
       </c>
       <c r="H131">
-        <v>60.253632402479752</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
+        <v>60.25363240247975</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
         <v>30</v>
       </c>
@@ -3631,12 +3610,12 @@
         <v>24.090906</v>
       </c>
       <c r="H132">
-        <v>60.230196406893121</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
+        <v>60.23019640689312</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
         <v>29</v>
       </c>
@@ -3653,12 +3632,12 @@
         <v>26.73753</v>
       </c>
       <c r="H133">
-        <v>60.214986201043999</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
+        <v>60.214986201044</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
         <v>30</v>
       </c>
@@ -3672,15 +3651,15 @@
         <v>1497</v>
       </c>
       <c r="G134">
-        <v>24.849015999999999</v>
+        <v>24.849016</v>
       </c>
       <c r="H134">
-        <v>60.243834202529378</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2" t="s">
+        <v>60.24383420252938</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -3699,12 +3678,12 @@
         <v>20.772879</v>
       </c>
       <c r="H135">
-        <v>60.270894564013012</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
+        <v>60.27089456401301</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
         <v>30</v>
       </c>
@@ -3718,15 +3697,15 @@
         <v>1222</v>
       </c>
       <c r="G136">
-        <v>20.266020999999999</v>
+        <v>20.266021</v>
       </c>
       <c r="H136">
-        <v>60.297973637745663</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
+        <v>60.29797363774566</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
         <v>29</v>
       </c>
@@ -3743,12 +3722,12 @@
         <v>21.351073</v>
       </c>
       <c r="H137">
-        <v>60.278001016623378</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
+        <v>60.27800101662338</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
         <v>30</v>
       </c>
@@ -3762,10 +3741,10 @@
         <v>1196</v>
       </c>
       <c r="G138">
-        <v>19.836376999999999</v>
+        <v>19.836377</v>
       </c>
       <c r="H138">
-        <v>60.293268271721189</v>
+        <v>60.29326827172119</v>
       </c>
     </row>
   </sheetData>
@@ -3806,15 +3785,21 @@
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B67:B70"/>
     <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B112"/>
     <mergeCell ref="B75:B78"/>
     <mergeCell ref="B79:B82"/>
     <mergeCell ref="B83:B86"/>
     <mergeCell ref="B87:B90"/>
     <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B112"/>
+    <mergeCell ref="B113:B117"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="B131:B134"/>
     <mergeCell ref="B135:B138"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
@@ -3825,21 +3810,15 @@
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="C124:C126"/>
-    <mergeCell ref="B113:B117"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="B127:B130"/>
-    <mergeCell ref="B131:B134"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="D124:D126"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="D124:D126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added alias infor to json file
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,11 @@
           <t>old fps</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -530,6 +535,11 @@
       </c>
       <c r="H2" t="n">
         <v>60</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -551,6 +561,11 @@
       <c r="H3" t="n">
         <v>60</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
@@ -578,6 +593,11 @@
       </c>
       <c r="H4" t="n">
         <v>60</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -599,6 +619,11 @@
       <c r="H5" t="n">
         <v>60</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -627,6 +652,11 @@
       <c r="H6" t="n">
         <v>60</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
@@ -655,6 +685,11 @@
       <c r="H7" t="n">
         <v>60</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -686,6 +721,11 @@
       </c>
       <c r="H8" t="n">
         <v>60</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -715,6 +755,11 @@
       <c r="H9" t="n">
         <v>60</v>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -743,6 +788,11 @@
       <c r="H10" t="n">
         <v>60</v>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -771,6 +821,11 @@
       <c r="H11" t="n">
         <v>60</v>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -806,6 +861,11 @@
       </c>
       <c r="H12" t="n">
         <v>60</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -835,6 +895,11 @@
       <c r="H13" t="n">
         <v>60</v>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
@@ -863,6 +928,11 @@
       <c r="H14" t="n">
         <v>60</v>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -891,6 +961,11 @@
       <c r="H15" t="n">
         <v>60</v>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
@@ -922,6 +997,11 @@
       </c>
       <c r="H16" t="n">
         <v>59</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -951,6 +1031,11 @@
       <c r="H17" t="n">
         <v>60</v>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
@@ -979,6 +1064,11 @@
       <c r="H18" t="n">
         <v>55.64724333807311</v>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
@@ -1007,6 +1097,11 @@
       <c r="H19" t="n">
         <v>54.24535307284484</v>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1042,6 +1137,11 @@
       </c>
       <c r="H20" t="n">
         <v>60</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1071,6 +1171,11 @@
       <c r="H21" t="n">
         <v>60</v>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
@@ -1099,6 +1204,11 @@
       <c r="H22" t="n">
         <v>60</v>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
@@ -1127,6 +1237,11 @@
       <c r="H23" t="n">
         <v>60</v>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -1158,6 +1273,11 @@
       </c>
       <c r="H24" t="n">
         <v>60</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1187,6 +1307,11 @@
       <c r="H25" t="n">
         <v>60</v>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
@@ -1215,6 +1340,11 @@
       <c r="H26" t="n">
         <v>60</v>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
@@ -1243,6 +1373,11 @@
       <c r="H27" t="n">
         <v>60</v>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1278,6 +1413,11 @@
       </c>
       <c r="H28" t="n">
         <v>60</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1307,6 +1447,11 @@
       <c r="H29" t="n">
         <v>60</v>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
@@ -1335,6 +1480,11 @@
       <c r="H30" t="n">
         <v>60</v>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
@@ -1363,6 +1513,11 @@
       <c r="H31" t="n">
         <v>60</v>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
@@ -1394,6 +1549,11 @@
       </c>
       <c r="H32" t="n">
         <v>60</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1423,6 +1583,11 @@
       <c r="H33" t="n">
         <v>60</v>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -1451,6 +1616,11 @@
       <c r="H34" t="n">
         <v>60</v>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
@@ -1479,6 +1649,11 @@
       <c r="H35" t="n">
         <v>60</v>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -1514,6 +1689,11 @@
       </c>
       <c r="H36" t="n">
         <v>60</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1543,6 +1723,11 @@
       <c r="H37" t="n">
         <v>60</v>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
@@ -1571,6 +1756,11 @@
       <c r="H38" t="n">
         <v>60</v>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
@@ -1599,6 +1789,11 @@
       <c r="H39" t="n">
         <v>60</v>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -1634,6 +1829,11 @@
       </c>
       <c r="H40" t="n">
         <v>60</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1655,6 +1855,11 @@
       <c r="H41" t="n">
         <v>60</v>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
@@ -1675,6 +1880,11 @@
       <c r="H42" t="n">
         <v>60</v>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
@@ -1703,6 +1913,11 @@
       <c r="H43" t="n">
         <v>60</v>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
@@ -1731,6 +1946,11 @@
       <c r="H44" t="n">
         <v>60</v>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
@@ -1759,6 +1979,11 @@
       <c r="H45" t="n">
         <v>60</v>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -1794,6 +2019,11 @@
       </c>
       <c r="H46" t="n">
         <v>59</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1823,6 +2053,11 @@
       <c r="H47" t="n">
         <v>44.82867396394455</v>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
@@ -1851,6 +2086,11 @@
       <c r="H48" t="n">
         <v>60</v>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
@@ -1879,6 +2119,11 @@
       <c r="H49" t="n">
         <v>60</v>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
@@ -1910,6 +2155,11 @@
       </c>
       <c r="H50" t="n">
         <v>60</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1931,6 +2181,11 @@
       <c r="H51" t="n">
         <v>60</v>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
@@ -1959,6 +2214,11 @@
       <c r="H52" t="n">
         <v>60</v>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
@@ -1986,6 +2246,11 @@
       </c>
       <c r="H53" t="n">
         <v>60</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -2007,6 +2272,11 @@
       <c r="H54" t="n">
         <v>60</v>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
@@ -2035,11 +2305,16 @@
       <c r="H55" t="n">
         <v>43.74386271896752</v>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Illia - 2</t>
+          <t>Illia2</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr">
@@ -2070,6 +2345,11 @@
       </c>
       <c r="H56" t="n">
         <v>60</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -2099,6 +2379,11 @@
       <c r="H57" t="n">
         <v>60</v>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
@@ -2126,6 +2411,11 @@
       </c>
       <c r="H58" t="n">
         <v>60</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -2147,6 +2437,11 @@
       <c r="H59" t="n">
         <v>59.94005994005994</v>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
@@ -2175,6 +2470,11 @@
       <c r="H60" t="n">
         <v>60</v>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
@@ -2206,6 +2506,11 @@
       </c>
       <c r="H61" t="n">
         <v>59.94005994005994</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -2235,6 +2540,11 @@
       <c r="H62" t="n">
         <v>60</v>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -2270,6 +2580,11 @@
       </c>
       <c r="H63" t="n">
         <v>60</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -2299,6 +2614,11 @@
       <c r="H64" t="n">
         <v>60</v>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
@@ -2327,6 +2647,11 @@
       <c r="H65" t="n">
         <v>60</v>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
@@ -2355,6 +2680,11 @@
       <c r="H66" t="n">
         <v>60</v>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
@@ -2386,6 +2716,11 @@
       </c>
       <c r="H67" t="n">
         <v>60</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -2415,6 +2750,11 @@
       <c r="H68" t="n">
         <v>60</v>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
@@ -2443,6 +2783,11 @@
       <c r="H69" t="n">
         <v>43.26212854125188</v>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
@@ -2471,6 +2816,11 @@
       <c r="H70" t="n">
         <v>60</v>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -2506,6 +2856,11 @@
       </c>
       <c r="H71" t="n">
         <v>60</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -2535,6 +2890,11 @@
       <c r="H72" t="n">
         <v>60</v>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
@@ -2563,6 +2923,11 @@
       <c r="H73" t="n">
         <v>60</v>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
@@ -2591,6 +2956,11 @@
       <c r="H74" t="n">
         <v>44.39181754032333</v>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
@@ -2622,6 +2992,11 @@
       </c>
       <c r="H75" t="n">
         <v>60</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -2651,6 +3026,11 @@
       <c r="H76" t="n">
         <v>60</v>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
@@ -2679,6 +3059,11 @@
       <c r="H77" t="n">
         <v>60</v>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
@@ -2707,6 +3092,11 @@
       <c r="H78" t="n">
         <v>60</v>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2742,6 +3132,11 @@
       </c>
       <c r="H79" t="n">
         <v>60</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -2771,6 +3166,11 @@
       <c r="H80" t="n">
         <v>60</v>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
@@ -2799,6 +3199,11 @@
       <c r="H81" t="n">
         <v>60</v>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
@@ -2827,6 +3232,11 @@
       <c r="H82" t="n">
         <v>60</v>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -2862,6 +3272,11 @@
       </c>
       <c r="H83" t="n">
         <v>60</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -2891,6 +3306,11 @@
       <c r="H84" t="n">
         <v>60</v>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
@@ -2919,6 +3339,11 @@
       <c r="H85" t="n">
         <v>60</v>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
@@ -2947,6 +3372,11 @@
       <c r="H86" t="n">
         <v>60</v>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
@@ -2978,6 +3408,11 @@
       </c>
       <c r="H87" t="n">
         <v>59</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -3007,6 +3442,11 @@
       <c r="H88" t="n">
         <v>60</v>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
@@ -3035,6 +3475,11 @@
       <c r="H89" t="n">
         <v>60</v>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
@@ -3063,6 +3508,11 @@
       <c r="H90" t="n">
         <v>60</v>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -3098,6 +3548,11 @@
       </c>
       <c r="H91" t="n">
         <v>60.25527302003672</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -3127,6 +3582,11 @@
       <c r="H92" t="n">
         <v>60</v>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
@@ -3158,6 +3618,11 @@
       </c>
       <c r="H93" t="n">
         <v>60</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="94">
@@ -3187,6 +3652,11 @@
       <c r="H94" t="n">
         <v>60</v>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
@@ -3215,6 +3685,11 @@
       <c r="H95" t="n">
         <v>60.28903363805564</v>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
@@ -3243,6 +3718,11 @@
       <c r="H96" t="n">
         <v>60</v>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
@@ -3278,6 +3758,11 @@
       </c>
       <c r="H97" t="n">
         <v>60</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -3307,6 +3792,11 @@
       <c r="H98" t="n">
         <v>60</v>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
@@ -3335,6 +3825,11 @@
       <c r="H99" t="n">
         <v>60</v>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
@@ -3363,6 +3858,11 @@
       <c r="H100" t="n">
         <v>60</v>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
@@ -3394,6 +3894,11 @@
       </c>
       <c r="H101" t="n">
         <v>60</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -3423,6 +3928,11 @@
       <c r="H102" t="n">
         <v>60</v>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
@@ -3451,6 +3961,11 @@
       <c r="H103" t="n">
         <v>60</v>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
@@ -3479,6 +3994,11 @@
       <c r="H104" t="n">
         <v>57.24750808541737</v>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
@@ -3514,6 +4034,11 @@
       </c>
       <c r="H105" t="n">
         <v>60</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="106">
@@ -3543,6 +4068,11 @@
       <c r="H106" t="n">
         <v>60</v>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n"/>
@@ -3571,6 +4101,11 @@
       <c r="H107" t="n">
         <v>60</v>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
@@ -3599,6 +4134,11 @@
       <c r="H108" t="n">
         <v>60</v>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n"/>
@@ -3630,6 +4170,11 @@
       </c>
       <c r="H109" t="n">
         <v>60</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="110">
@@ -3659,6 +4204,11 @@
       <c r="H110" t="n">
         <v>60</v>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
@@ -3687,6 +4237,11 @@
       <c r="H111" t="n">
         <v>60</v>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
@@ -3715,6 +4270,11 @@
       <c r="H112" t="n">
         <v>60</v>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
@@ -3750,6 +4310,11 @@
       </c>
       <c r="H113" t="n">
         <v>59.94005994005994</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="114">
@@ -3779,6 +4344,11 @@
       <c r="H114" t="n">
         <v>60</v>
       </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n"/>
@@ -3807,6 +4377,11 @@
       <c r="H115" t="n">
         <v>59.94005994005994</v>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
@@ -3834,6 +4409,11 @@
       </c>
       <c r="H116" t="n">
         <v>34.00105420527455</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -3855,6 +4435,11 @@
       <c r="H117" t="n">
         <v>60.08833797308407</v>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
@@ -3886,6 +4471,11 @@
       </c>
       <c r="H118" t="n">
         <v>60</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="119">
@@ -3915,6 +4505,11 @@
       <c r="H119" t="n">
         <v>60</v>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
@@ -3943,6 +4538,11 @@
       <c r="H120" t="n">
         <v>60</v>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n"/>
@@ -3971,6 +4571,11 @@
       <c r="H121" t="n">
         <v>60</v>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
@@ -4006,6 +4611,11 @@
       </c>
       <c r="H122" t="n">
         <v>60</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
     </row>
     <row r="123">
@@ -4027,6 +4637,11 @@
       <c r="H123" t="n">
         <v>60</v>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
@@ -4054,6 +4669,11 @@
       </c>
       <c r="H124" t="n">
         <v>60.44279297908365</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
     </row>
     <row r="125">
@@ -4075,6 +4695,11 @@
       <c r="H125" t="n">
         <v>60.45196735593763</v>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
@@ -4095,6 +4720,11 @@
       <c r="H126" t="n">
         <v>60</v>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
@@ -4130,6 +4760,11 @@
       </c>
       <c r="H127" t="n">
         <v>60</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="128">
@@ -4159,6 +4794,11 @@
       <c r="H128" t="n">
         <v>60</v>
       </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
@@ -4187,6 +4827,11 @@
       <c r="H129" t="n">
         <v>60</v>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
@@ -4215,6 +4860,11 @@
       <c r="H130" t="n">
         <v>60</v>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
@@ -4250,6 +4900,11 @@
       </c>
       <c r="H131" t="n">
         <v>60</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="132">
@@ -4279,6 +4934,11 @@
       <c r="H132" t="n">
         <v>60</v>
       </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
@@ -4307,6 +4967,11 @@
       <c r="H133" t="n">
         <v>60</v>
       </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
@@ -4335,6 +5000,11 @@
       <c r="H134" t="n">
         <v>60.24383420252938</v>
       </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n"/>
@@ -4366,6 +5036,11 @@
       </c>
       <c r="H135" t="n">
         <v>60.27089456401301</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="136">
@@ -4395,6 +5070,11 @@
       <c r="H136" t="n">
         <v>60</v>
       </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n"/>
@@ -4423,6 +5103,11 @@
       <c r="H137" t="n">
         <v>60</v>
       </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n"/>
@@ -4450,6 +5135,11 @@
       </c>
       <c r="H138" t="n">
         <v>60</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed no alias bug
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -4614,7 +4614,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added extract info from filepath
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1664,1007 +1664,28 @@
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>Jay</t>
-        </is>
-      </c>
-      <c r="B37" s="1" t="inlineStr">
-        <is>
-          <t>2 Meters</t>
-        </is>
-      </c>
-      <c r="C37" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D37" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E37" s="1" t="inlineStr">
-        <is>
-          <t>Jay HB.mp4</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>1699</v>
-      </c>
-      <c r="G37" t="n">
-        <v>39.857232</v>
-      </c>
-      <c r="H37" t="n">
-        <v>42.62714480523886</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n"/>
-      <c r="C38" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D38" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E38" s="1" t="inlineStr">
-        <is>
-          <t>Jay.mp4</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>1609</v>
-      </c>
-      <c r="G38" t="n">
-        <v>36.617027</v>
-      </c>
-      <c r="H38" t="n">
-        <v>43.94130632178303</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n"/>
-      <c r="C39" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D39" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E39" s="1" t="inlineStr">
-        <is>
-          <t>Jay HB.mp4</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>2229</v>
-      </c>
-      <c r="G39" t="n">
-        <v>46.20177</v>
-      </c>
-      <c r="H39" t="n">
-        <v>48.24490490299397</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n"/>
-      <c r="B40" s="1" t="n"/>
-      <c r="C40" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D40" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E40" s="1" t="inlineStr">
-        <is>
-          <t>Jay.mp4</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>1697</v>
-      </c>
-      <c r="G40" t="n">
-        <v>31.0855</v>
-      </c>
-      <c r="H40" t="n">
-        <v>54.59136896623828</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="inlineStr">
-        <is>
-          <t>3 Meters</t>
-        </is>
-      </c>
-      <c r="C41" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D41" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E41" s="1" t="inlineStr">
-        <is>
-          <t>Jay HB.mp4</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>1668</v>
-      </c>
-      <c r="G41" t="n">
-        <v>36.827158</v>
-      </c>
-      <c r="H41" t="n">
-        <v>45.29266146467235</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D42" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E42" s="1" t="inlineStr">
-        <is>
-          <t>Jay.mp4</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>1616</v>
-      </c>
-      <c r="G42" t="n">
-        <v>35.511938</v>
-      </c>
-      <c r="H42" t="n">
-        <v>45.5058239851624</v>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n"/>
-      <c r="C43" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D43" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E43" s="1" t="inlineStr">
-        <is>
-          <t>Jay HB.mp4</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>1846</v>
-      </c>
-      <c r="G43" t="n">
-        <v>42.670115</v>
-      </c>
-      <c r="H43" t="n">
-        <v>43.26212854125188</v>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="n"/>
-      <c r="C44" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D44" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E44" s="1" t="inlineStr">
-        <is>
-          <t>Jay.mp4</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>1760</v>
-      </c>
-      <c r="G44" t="n">
-        <v>39.149083</v>
-      </c>
-      <c r="H44" t="n">
-        <v>44.9563531283734</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Joseph</t>
-        </is>
-      </c>
-      <c r="B45" s="1" t="inlineStr">
-        <is>
-          <t>2 Meters</t>
-        </is>
-      </c>
-      <c r="C45" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D45" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E45" s="1" t="inlineStr">
-        <is>
-          <t>Joseph HB.mp4</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>1434</v>
-      </c>
-      <c r="G45" t="n">
-        <v>28.500216</v>
-      </c>
-      <c r="H45" t="n">
-        <v>50.31540813585413</v>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n"/>
-      <c r="C46" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D46" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E46" s="1" t="inlineStr">
-        <is>
-          <t>Joseph.mp4</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
-        <v>1450</v>
-      </c>
-      <c r="G46" t="n">
-        <v>28.554858</v>
-      </c>
-      <c r="H46" t="n">
-        <v>50.77945055794009</v>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n"/>
-      <c r="C47" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D47" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E47" s="1" t="inlineStr">
-        <is>
-          <t>Joseph HB.mp4</t>
-        </is>
-      </c>
-      <c r="F47" t="n">
-        <v>1505</v>
-      </c>
-      <c r="G47" t="n">
-        <v>28.038409</v>
-      </c>
-      <c r="H47" t="n">
-        <v>53.67636944022038</v>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n"/>
-      <c r="B48" s="1" t="n"/>
-      <c r="C48" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D48" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E48" s="1" t="inlineStr">
-        <is>
-          <t>Joseph.mp4</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
-        <v>1487</v>
-      </c>
-      <c r="G48" t="n">
-        <v>28.196682</v>
-      </c>
-      <c r="H48" t="n">
-        <v>52.73670143175002</v>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Melissa</t>
-        </is>
-      </c>
-      <c r="B49" s="1" t="inlineStr">
-        <is>
-          <t>2 Meters</t>
-        </is>
-      </c>
-      <c r="C49" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D49" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E49" s="1" t="inlineStr">
-        <is>
-          <t>Melissa HB.mp4</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>2525</v>
-      </c>
-      <c r="G49" t="n">
-        <v>46.704064</v>
-      </c>
-      <c r="H49" t="n">
-        <v>54.06381765835196</v>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n"/>
-      <c r="C50" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D50" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E50" s="1" t="inlineStr">
-        <is>
-          <t>Melissa.mp4</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
-        <v>3569</v>
-      </c>
-      <c r="G50" t="n">
-        <v>64.145798</v>
-      </c>
-      <c r="H50" t="n">
-        <v>55.63887442790875</v>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="n"/>
-      <c r="C51" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D51" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E51" s="1" t="inlineStr">
-        <is>
-          <t>Melissa HB.mp4</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
-        <v>2786</v>
-      </c>
-      <c r="G51" t="n">
-        <v>57.93909</v>
-      </c>
-      <c r="H51" t="n">
-        <v>48.08498027842688</v>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n"/>
-      <c r="C52" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D52" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E52" s="1" t="inlineStr">
-        <is>
-          <t>Melissa.mp4</t>
-        </is>
-      </c>
-      <c r="F52" t="n">
-        <v>3111</v>
-      </c>
-      <c r="G52" t="n">
-        <v>66.993945</v>
-      </c>
-      <c r="H52" t="n">
-        <v>46.43703248106974</v>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="inlineStr">
-        <is>
-          <t>3 Meters</t>
-        </is>
-      </c>
-      <c r="C53" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D53" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E53" s="1" t="inlineStr">
-        <is>
-          <t>Melissa HB.mp4</t>
-        </is>
-      </c>
-      <c r="F53" t="n">
-        <v>2606</v>
-      </c>
-      <c r="G53" t="n">
-        <v>50.591942</v>
-      </c>
-      <c r="H53" t="n">
-        <v>51.51017922972792</v>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D54" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E54" s="1" t="inlineStr">
-        <is>
-          <t>Melissa.mp4</t>
-        </is>
-      </c>
-      <c r="F54" t="n">
-        <v>2821</v>
-      </c>
-      <c r="G54" t="n">
-        <v>53.759293</v>
-      </c>
-      <c r="H54" t="n">
-        <v>52.47464842962128</v>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n"/>
-      <c r="C55" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D55" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E55" s="1" t="inlineStr">
-        <is>
-          <t>Melissa HB.mp4</t>
-        </is>
-      </c>
-      <c r="F55" t="n">
-        <v>2760</v>
-      </c>
-      <c r="G55" t="n">
-        <v>52.458189</v>
-      </c>
-      <c r="H55" t="n">
-        <v>52.61332982730303</v>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n"/>
-      <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D56" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E56" s="1" t="inlineStr">
-        <is>
-          <t>Melissa.mp4</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
-        <v>2517</v>
-      </c>
-      <c r="G56" t="n">
-        <v>48.236838</v>
-      </c>
-      <c r="H56" t="n">
-        <v>52.18003717407845</v>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Sara</t>
-        </is>
-      </c>
-      <c r="B57" s="1" t="inlineStr">
-        <is>
-          <t>2 Meters</t>
-        </is>
-      </c>
-      <c r="C57" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D57" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E57" s="1" t="inlineStr">
-        <is>
-          <t>Sara HB.mp4</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
-        <v>1328</v>
-      </c>
-      <c r="G57" t="n">
-        <v>22.040165</v>
-      </c>
-      <c r="H57" t="n">
-        <v>60.25363240247975</v>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="n"/>
-      <c r="C58" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D58" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E58" s="1" t="inlineStr">
-        <is>
-          <t>Sara Relaxed with Blanket.mp4</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
-        <v>1451</v>
-      </c>
-      <c r="G58" t="n">
-        <v>24.090906</v>
-      </c>
-      <c r="H58" t="n">
-        <v>60.23019640689312</v>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="n"/>
-      <c r="C59" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D59" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E59" s="1" t="inlineStr">
-        <is>
-          <t>Sara Hold Breath.mp4</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
-        <v>1610</v>
-      </c>
-      <c r="G59" t="n">
-        <v>26.73753</v>
-      </c>
-      <c r="H59" t="n">
-        <v>60.214986201044</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="n"/>
-      <c r="C60" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D60" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E60" s="1" t="inlineStr">
-        <is>
-          <t>Sara Relaxed.mp4</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>1497</v>
-      </c>
-      <c r="G60" t="n">
-        <v>24.849016</v>
-      </c>
-      <c r="H60" t="n">
-        <v>60.24383420252938</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="inlineStr">
-        <is>
-          <t>3 Meters</t>
-        </is>
-      </c>
-      <c r="C61" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D61" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E61" s="1" t="inlineStr">
-        <is>
-          <t>Sara HB.mp4</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
-        <v>1252</v>
-      </c>
-      <c r="G61" t="n">
-        <v>20.772879</v>
-      </c>
-      <c r="H61" t="n">
-        <v>60.27089456401301</v>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n"/>
-      <c r="C62" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D62" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E62" s="1" t="inlineStr">
-        <is>
-          <t>Sara Relaxed.mp4</t>
-        </is>
-      </c>
-      <c r="F62" t="n">
-        <v>1222</v>
-      </c>
-      <c r="G62" t="n">
-        <v>20.266021</v>
-      </c>
-      <c r="H62" t="n">
-        <v>60.29797363774566</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="n"/>
-      <c r="C63" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D63" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E63" s="1" t="inlineStr">
-        <is>
-          <t>Sara HB.mp4</t>
-        </is>
-      </c>
-      <c r="F63" t="n">
-        <v>1287</v>
-      </c>
-      <c r="G63" t="n">
-        <v>21.351073</v>
-      </c>
-      <c r="H63" t="n">
-        <v>60.27800101662338</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n"/>
-      <c r="B64" s="1" t="n"/>
-      <c r="C64" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D64" s="1" t="inlineStr">
-        <is>
-          <t>Without Blankets</t>
-        </is>
-      </c>
-      <c r="E64" s="1" t="inlineStr">
-        <is>
-          <t>Sara Relaxed.mp4</t>
-        </is>
-      </c>
-      <c r="F64" t="n">
-        <v>1196</v>
-      </c>
-      <c r="G64" t="n">
-        <v>19.836377</v>
-      </c>
-      <c r="H64" t="n">
-        <v>60.29326827172119</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="22">
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="A20:A29"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A49:A56"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B61:B64"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B57:B60"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B53:B56"/>
     <mergeCell ref="A12:A19"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A44"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B49:B52"/>
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="B24:B29"/>
-    <mergeCell ref="A57:A64"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B45:B48"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="B35:B36"/>
   </mergeCells>

</xml_diff>

<commit_message>
added script to validate run
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,7 +830,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Eddy</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -850,21 +850,21 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>Eddy HB.mp4</t>
+          <t>Daniel HB.mp4</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2495</v>
+        <v>2582</v>
       </c>
       <c r="G12" t="n">
-        <v>56.954748</v>
+        <v>48.922989</v>
       </c>
       <c r="H12" t="n">
-        <v>43.806707739274</v>
+        <v>52.77682440866399</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -883,21 +883,21 @@
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>Eddy.mp4</t>
+          <t>Daniel.mp4</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2501</v>
+        <v>3145</v>
       </c>
       <c r="G13" t="n">
-        <v>57.296129</v>
+        <v>60.784128</v>
       </c>
       <c r="H13" t="n">
-        <v>43.65041833803467</v>
+        <v>51.74048067284933</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -916,21 +916,21 @@
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>Eddy HB.mp4</t>
+          <t>Daniel HB.mp4</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2656</v>
+        <v>2578</v>
       </c>
       <c r="G14" t="n">
-        <v>48.1372</v>
+        <v>61.6722</v>
       </c>
       <c r="H14" t="n">
-        <v>55.17562301089387</v>
+        <v>41.80165455424</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -949,21 +949,21 @@
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>Eddy.mp4</t>
+          <t>Daniel.mp4</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2686</v>
+        <v>2704</v>
       </c>
       <c r="G15" t="n">
-        <v>48.899545</v>
+        <v>63.79880499999999</v>
       </c>
       <c r="H15" t="n">
-        <v>54.9289364553392</v>
+        <v>42.3832389964044</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -986,21 +986,21 @@
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>Eddy HB.mp4</t>
+          <t>Daniel HB.mp4</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1506</v>
+        <v>1188</v>
       </c>
       <c r="G16" t="n">
-        <v>27.845039</v>
+        <v>26.326683</v>
       </c>
       <c r="H16" t="n">
-        <v>54.08503827198805</v>
+        <v>45.12532019320474</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1019,21 +1019,21 @@
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>Eddy.mp4</t>
+          <t>Daniel.mp4</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1540</v>
+        <v>1279</v>
       </c>
       <c r="G17" t="n">
-        <v>29.567784</v>
+        <v>29.29561</v>
       </c>
       <c r="H17" t="n">
-        <v>52.08371381500893</v>
+        <v>43.65841844563059</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1052,21 +1052,21 @@
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>Eddy HB.mp4</t>
+          <t>Daniel HB.mp4</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1519</v>
+        <v>1406</v>
       </c>
       <c r="G18" t="n">
-        <v>29.396478</v>
+        <v>25.266301</v>
       </c>
       <c r="H18" t="n">
-        <v>51.67285686400935</v>
+        <v>55.64724333807311</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1085,28 +1085,28 @@
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>Eddy.mp4</t>
+          <t>Daniel.mp4</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1487</v>
+        <v>1335</v>
       </c>
       <c r="G19" t="n">
-        <v>31.277956</v>
+        <v>24.610403</v>
       </c>
       <c r="H19" t="n">
-        <v>47.54146978146526</v>
+        <v>54.24535307284484</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Illia</t>
+          <t>Eddy</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -1126,21 +1126,21 @@
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>Illia HB.mp4</t>
+          <t>Eddy HB.mp4</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1997</v>
+        <v>2495</v>
       </c>
       <c r="G20" t="n">
-        <v>42.697471</v>
+        <v>56.954748</v>
       </c>
       <c r="H20" t="n">
-        <v>46.77091999195924</v>
+        <v>43.806707739274</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1159,21 +1159,21 @@
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>Illia.mp4</t>
+          <t>Eddy.mp4</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>2311</v>
+        <v>2501</v>
       </c>
       <c r="G21" t="n">
-        <v>51.55182600000001</v>
+        <v>57.296129</v>
       </c>
       <c r="H21" t="n">
-        <v>44.82867396394455</v>
+        <v>43.65041833803467</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1192,21 +1192,21 @@
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>Illia HB.mp4</t>
+          <t>Eddy HB.mp4</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2154</v>
+        <v>2656</v>
       </c>
       <c r="G22" t="n">
-        <v>40.820155</v>
+        <v>48.1372</v>
       </c>
       <c r="H22" t="n">
-        <v>52.76805048878428</v>
+        <v>55.17562301089387</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1225,21 +1225,21 @@
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>Illia.mp4</t>
+          <t>Eddy.mp4</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2442</v>
+        <v>2686</v>
       </c>
       <c r="G23" t="n">
-        <v>49.465783</v>
+        <v>48.899545</v>
       </c>
       <c r="H23" t="n">
-        <v>49.36745871383457</v>
+        <v>54.9289364553392</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1262,46 +1262,54 @@
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>Illia HB.mp4</t>
+          <t>Eddy HB.mp4</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>4088</v>
+        <v>1506</v>
       </c>
       <c r="G24" t="n">
-        <v>82.335533</v>
+        <v>27.845039</v>
       </c>
       <c r="H24" t="n">
-        <v>49.65049536996378</v>
+        <v>54.08503827198805</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="n"/>
-      <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n"/>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>Illia HB2.mp4</t>
+          <t>Eddy.mp4</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>3955</v>
+        <v>1540</v>
       </c>
       <c r="G25" t="n">
-        <v>81.783652</v>
+        <v>29.567784</v>
       </c>
       <c r="H25" t="n">
-        <v>48.35929801716362</v>
+        <v>52.08371381500893</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1310,31 +1318,31 @@
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>Relaxed</t>
+          <t>Hold Breath</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>With Blankets</t>
+          <t>Without Blankets</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>Illia.mp4</t>
+          <t>Eddy HB.mp4</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2808</v>
+        <v>1519</v>
       </c>
       <c r="G26" t="n">
-        <v>57.00986900000001</v>
+        <v>29.396478</v>
       </c>
       <c r="H26" t="n">
-        <v>49.25462993082829</v>
+        <v>51.67285686400935</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1351,7 @@
       <c r="B27" s="1" t="n"/>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>Hold Breath</t>
+          <t>Relaxed</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
@@ -1353,46 +1361,62 @@
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>Illia HB.mp4</t>
+          <t>Eddy.mp4</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2290</v>
+        <v>1487</v>
       </c>
       <c r="G27" t="n">
-        <v>53.05520600000001</v>
+        <v>31.277956</v>
       </c>
       <c r="H27" t="n">
-        <v>43.16258804084183</v>
+        <v>47.54146978146526</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n"/>
-      <c r="C28" s="1" t="n"/>
-      <c r="D28" s="1" t="n"/>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Farooq</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>Illia HB1.mp4</t>
+          <t>Farooq.mp4</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1740</v>
+        <v>1682</v>
       </c>
       <c r="G28" t="n">
-        <v>38.47498</v>
+        <v>31.644664</v>
       </c>
       <c r="H28" t="n">
-        <v>45.22419504831451</v>
+        <v>53.15272110331144</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -1406,40 +1430,32 @@
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>Without Blankets</t>
+          <t>With Blankets</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>Illia.mp4</t>
+          <t>Farooq.mp4</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>3071</v>
+        <v>1457</v>
       </c>
       <c r="G29" t="n">
-        <v>70.204134</v>
+        <v>28.055417</v>
       </c>
       <c r="H29" t="n">
-        <v>43.74386271896752</v>
+        <v>51.93292974401343</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Illia2</t>
-        </is>
-      </c>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>2 Meters</t>
-        </is>
-      </c>
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="inlineStr">
         <is>
           <t>Hold Breath</t>
@@ -1447,26 +1463,26 @@
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>With Blankets</t>
+          <t>Without Blankets</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>Illia2 HB.mp4</t>
+          <t>Farooq HB.mp4</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1497</v>
+        <v>1511</v>
       </c>
       <c r="G30" t="n">
-        <v>27.849945</v>
+        <v>30.413066</v>
       </c>
       <c r="H30" t="n">
-        <v>53.75235031882469</v>
+        <v>49.68259365892278</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -1480,32 +1496,36 @@
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>With Blankets</t>
+          <t>Without Blankets</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>Illia2.mp4</t>
+          <t>Farooq.mp4</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1664</v>
+        <v>3665</v>
       </c>
       <c r="G31" t="n">
-        <v>32.986516</v>
+        <v>77.43016</v>
       </c>
       <c r="H31" t="n">
-        <v>50.4448544975165</v>
+        <v>47.33297722747829</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
           <t>Hold Breath</t>
@@ -1513,51 +1533,59 @@
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
-          <t>Without Blankets</t>
+          <t>With Blankets</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>Iliia2 HB.mp4</t>
+          <t>Farooq HB.mp4</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1299</v>
+        <v>1537</v>
       </c>
       <c r="G32" t="n">
-        <v>27.687303</v>
+        <v>37.05066</v>
       </c>
       <c r="H32" t="n">
-        <v>46.91681237424967</v>
+        <v>41.48374145021978</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
-      <c r="D33" s="1" t="n"/>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>Iliia3 HB.mp4</t>
+          <t>Farooq.mp4</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>8111</v>
+        <v>1563</v>
       </c>
       <c r="G33" t="n">
-        <v>161.407619</v>
+        <v>36.911795</v>
       </c>
       <c r="H33" t="n">
-        <v>50.25165509690097</v>
+        <v>42.34418835496892</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1594,7 @@
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>Relaxed</t>
+          <t>Hold Breath</t>
         </is>
       </c>
       <c r="D34" s="1" t="inlineStr">
@@ -1576,118 +1604,3616 @@
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>Illia2.mp4</t>
+          <t>Farooq HB.mp4</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>2335</v>
+        <v>1867</v>
       </c>
       <c r="G34" t="n">
-        <v>52.505819</v>
+        <v>45.610873</v>
       </c>
       <c r="H34" t="n">
-        <v>44.4712613662878</v>
+        <v>40.9332222165535</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
-      <c r="B35" s="1" t="inlineStr">
+      <c r="B35" s="1" t="n"/>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>Farooq.mp4</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>3217</v>
+      </c>
+      <c r="G35" t="n">
+        <v>74.95078000000001</v>
+      </c>
+      <c r="H35" t="n">
+        <v>42.92150128390925</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Frank</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>Frank HB.mp4</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1830</v>
+      </c>
+      <c r="G36" t="n">
+        <v>36.819093</v>
+      </c>
+      <c r="H36" t="n">
+        <v>49.70247365952225</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="n"/>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>Frank.mp4</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>2103</v>
+      </c>
+      <c r="G37" t="n">
+        <v>39.155347</v>
+      </c>
+      <c r="H37" t="n">
+        <v>53.70913964828354</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="n"/>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>Frank HB.mp4</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>2176</v>
+      </c>
+      <c r="G38" t="n">
+        <v>45.652923</v>
+      </c>
+      <c r="H38" t="n">
+        <v>47.66397980694467</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>Frank.mp4</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1909</v>
+      </c>
+      <c r="G39" t="n">
+        <v>40.17193</v>
+      </c>
+      <c r="H39" t="n">
+        <v>47.5207439622642</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Frank2</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
         <is>
           <t>3 Meters</t>
         </is>
       </c>
-      <c r="C35" s="1" t="inlineStr">
-        <is>
-          <t>Hold Breath</t>
-        </is>
-      </c>
-      <c r="D35" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E35" s="1" t="inlineStr">
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>Frank2 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1536</v>
+      </c>
+      <c r="G40" t="n">
+        <v>27.354892</v>
+      </c>
+      <c r="H40" t="n">
+        <v>56.15083400804507</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n"/>
+      <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
+      <c r="D41" s="1" t="n"/>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>Frank3 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1413</v>
+      </c>
+      <c r="G41" t="n">
+        <v>27.097133</v>
+      </c>
+      <c r="H41" t="n">
+        <v>52.1457380749469</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="1" t="n"/>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>Frank4 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1420</v>
+      </c>
+      <c r="G42" t="n">
+        <v>27.617738</v>
+      </c>
+      <c r="H42" t="n">
+        <v>51.41623111929007</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n"/>
+      <c r="B43" s="1" t="n"/>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>Frank2.mp4</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1460</v>
+      </c>
+      <c r="G43" t="n">
+        <v>26.896963</v>
+      </c>
+      <c r="H43" t="n">
+        <v>54.28122126650507</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>Frank2 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1564</v>
+      </c>
+      <c r="G44" t="n">
+        <v>28.472678</v>
+      </c>
+      <c r="H44" t="n">
+        <v>54.92985240095786</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n"/>
+      <c r="B45" s="1" t="n"/>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>Frank2.mp4</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>1713</v>
+      </c>
+      <c r="G45" t="n">
+        <v>31.041202</v>
+      </c>
+      <c r="H45" t="n">
+        <v>55.18471868454063</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Illia</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB.mp4</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1997</v>
+      </c>
+      <c r="G46" t="n">
+        <v>42.697471</v>
+      </c>
+      <c r="H46" t="n">
+        <v>46.77091999195924</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n"/>
+      <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>Illia.mp4</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>2311</v>
+      </c>
+      <c r="G47" t="n">
+        <v>51.55182600000001</v>
+      </c>
+      <c r="H47" t="n">
+        <v>44.82867396394455</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n"/>
+      <c r="B48" s="1" t="n"/>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB.mp4</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>2154</v>
+      </c>
+      <c r="G48" t="n">
+        <v>40.820155</v>
+      </c>
+      <c r="H48" t="n">
+        <v>52.76805048878428</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n"/>
+      <c r="B49" s="1" t="n"/>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>Illia.mp4</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>2442</v>
+      </c>
+      <c r="G49" t="n">
+        <v>49.465783</v>
+      </c>
+      <c r="H49" t="n">
+        <v>49.36745871383457</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n"/>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB.mp4</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>4088</v>
+      </c>
+      <c r="G50" t="n">
+        <v>82.335533</v>
+      </c>
+      <c r="H50" t="n">
+        <v>49.65049536996378</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n"/>
+      <c r="B51" s="1" t="n"/>
+      <c r="C51" s="1" t="n"/>
+      <c r="D51" s="1" t="n"/>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB2.mp4</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>3955</v>
+      </c>
+      <c r="G51" t="n">
+        <v>81.783652</v>
+      </c>
+      <c r="H51" t="n">
+        <v>48.35929801716362</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n"/>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D52" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>Illia.mp4</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>2808</v>
+      </c>
+      <c r="G52" t="n">
+        <v>57.00986900000001</v>
+      </c>
+      <c r="H52" t="n">
+        <v>49.25462993082829</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n"/>
+      <c r="B53" s="1" t="n"/>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB.mp4</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>2290</v>
+      </c>
+      <c r="G53" t="n">
+        <v>53.05520600000001</v>
+      </c>
+      <c r="H53" t="n">
+        <v>43.16258804084183</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n"/>
+      <c r="B54" s="1" t="n"/>
+      <c r="C54" s="1" t="n"/>
+      <c r="D54" s="1" t="n"/>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>Illia HB1.mp4</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>1740</v>
+      </c>
+      <c r="G54" t="n">
+        <v>38.47498</v>
+      </c>
+      <c r="H54" t="n">
+        <v>45.22419504831451</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n"/>
+      <c r="B55" s="1" t="n"/>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>Illia.mp4</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>3071</v>
+      </c>
+      <c r="G55" t="n">
+        <v>70.204134</v>
+      </c>
+      <c r="H55" t="n">
+        <v>43.74386271896752</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Illia2</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>Illia2 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>1497</v>
+      </c>
+      <c r="G56" t="n">
+        <v>27.849945</v>
+      </c>
+      <c r="H56" t="n">
+        <v>53.75235031882469</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n"/>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>Illia2.mp4</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>1664</v>
+      </c>
+      <c r="G57" t="n">
+        <v>32.986516</v>
+      </c>
+      <c r="H57" t="n">
+        <v>50.4448544975165</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n"/>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>Iliia2 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1299</v>
+      </c>
+      <c r="G58" t="n">
+        <v>27.687303</v>
+      </c>
+      <c r="H58" t="n">
+        <v>46.91681237424967</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n"/>
+      <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>Iliia3 HB.mp4</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>8111</v>
+      </c>
+      <c r="G59" t="n">
+        <v>161.407619</v>
+      </c>
+      <c r="H59" t="n">
+        <v>50.25165509690097</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n"/>
+      <c r="B60" s="1" t="n"/>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>Illia2.mp4</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>2335</v>
+      </c>
+      <c r="G60" t="n">
+        <v>52.505819</v>
+      </c>
+      <c r="H60" t="n">
+        <v>44.4712613662878</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n"/>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D61" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E61" s="1" t="inlineStr">
         <is>
           <t>Illia4 HB.mp4</t>
         </is>
       </c>
-      <c r="F35" t="n">
+      <c r="F61" t="n">
         <v>1671</v>
       </c>
-      <c r="G35" t="n">
+      <c r="G61" t="n">
         <v>30.828421</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H61" t="n">
         <v>54.20323019463112</v>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="I61" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n"/>
-      <c r="C36" s="1" t="inlineStr">
-        <is>
-          <t>Relaxed</t>
-        </is>
-      </c>
-      <c r="D36" s="1" t="inlineStr">
-        <is>
-          <t>With Blankets</t>
-        </is>
-      </c>
-      <c r="E36" s="1" t="inlineStr">
+    <row r="62">
+      <c r="A62" s="1" t="n"/>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D62" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr">
         <is>
           <t>Illia4.mp4</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="F62" t="n">
         <v>1440</v>
       </c>
-      <c r="G36" t="n">
+      <c r="G62" t="n">
         <v>26.348691</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H62" t="n">
         <v>54.65167131073039</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="I62" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>Jay</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D63" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>Jay HB.mp4</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>1699</v>
+      </c>
+      <c r="G63" t="n">
+        <v>39.857232</v>
+      </c>
+      <c r="H63" t="n">
+        <v>42.62714480523886</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D64" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>Jay.mp4</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>1609</v>
+      </c>
+      <c r="G64" t="n">
+        <v>36.617027</v>
+      </c>
+      <c r="H64" t="n">
+        <v>43.94130632178303</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n"/>
+      <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>Jay HB.mp4</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>2229</v>
+      </c>
+      <c r="G65" t="n">
+        <v>46.20177</v>
+      </c>
+      <c r="H65" t="n">
+        <v>48.24490490299397</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n"/>
+      <c r="B66" s="1" t="n"/>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>Jay.mp4</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1697</v>
+      </c>
+      <c r="G66" t="n">
+        <v>31.0855</v>
+      </c>
+      <c r="H66" t="n">
+        <v>54.59136896623828</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n"/>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D67" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E67" s="1" t="inlineStr">
+        <is>
+          <t>Jay HB.mp4</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1668</v>
+      </c>
+      <c r="G67" t="n">
+        <v>36.827158</v>
+      </c>
+      <c r="H67" t="n">
+        <v>45.29266146467235</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n"/>
+      <c r="B68" s="1" t="n"/>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D68" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E68" s="1" t="inlineStr">
+        <is>
+          <t>Jay.mp4</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1616</v>
+      </c>
+      <c r="G68" t="n">
+        <v>35.511938</v>
+      </c>
+      <c r="H68" t="n">
+        <v>45.5058239851624</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n"/>
+      <c r="B69" s="1" t="n"/>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D69" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E69" s="1" t="inlineStr">
+        <is>
+          <t>Jay HB.mp4</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>1846</v>
+      </c>
+      <c r="G69" t="n">
+        <v>42.670115</v>
+      </c>
+      <c r="H69" t="n">
+        <v>43.26212854125188</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n"/>
+      <c r="B70" s="1" t="n"/>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D70" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E70" s="1" t="inlineStr">
+        <is>
+          <t>Jay.mp4</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>1760</v>
+      </c>
+      <c r="G70" t="n">
+        <v>39.149083</v>
+      </c>
+      <c r="H70" t="n">
+        <v>44.9563531283734</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D71" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E71" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil HB.mp4</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>1438</v>
+      </c>
+      <c r="G71" t="n">
+        <v>34.130222</v>
+      </c>
+      <c r="H71" t="n">
+        <v>42.13274674861476</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n"/>
+      <c r="B72" s="1" t="n"/>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D72" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E72" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil.mp4</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1446</v>
+      </c>
+      <c r="G72" t="n">
+        <v>32.73897299999999</v>
+      </c>
+      <c r="H72" t="n">
+        <v>44.16754306862344</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n"/>
+      <c r="B73" s="1" t="n"/>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D73" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E73" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil HB.mp4</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>1525</v>
+      </c>
+      <c r="G73" t="n">
+        <v>33.163763</v>
+      </c>
+      <c r="H73" t="n">
+        <v>45.98392528616249</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n"/>
+      <c r="B74" s="1" t="n"/>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D74" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E74" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil.mp4</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>1555</v>
+      </c>
+      <c r="G74" t="n">
+        <v>35.028978</v>
+      </c>
+      <c r="H74" t="n">
+        <v>44.39181754032333</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n"/>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D75" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E75" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil HB.mp4</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>1612</v>
+      </c>
+      <c r="G75" t="n">
+        <v>31.664546</v>
+      </c>
+      <c r="H75" t="n">
+        <v>50.90867243130535</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n"/>
+      <c r="B76" s="1" t="n"/>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D76" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E76" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil.mp4</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>1613</v>
+      </c>
+      <c r="G76" t="n">
+        <v>31.912436</v>
+      </c>
+      <c r="H76" t="n">
+        <v>50.54455886727042</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n"/>
+      <c r="B77" s="1" t="n"/>
+      <c r="C77" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D77" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E77" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil HB.mp4</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>1632</v>
+      </c>
+      <c r="G77" t="n">
+        <v>36.441915</v>
+      </c>
+      <c r="H77" t="n">
+        <v>44.78359603220632</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n"/>
+      <c r="B78" s="1" t="n"/>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D78" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E78" s="1" t="inlineStr">
+        <is>
+          <t>John McNeil.mp4</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>1617</v>
+      </c>
+      <c r="G78" t="n">
+        <v>34.73233099999999</v>
+      </c>
+      <c r="H78" t="n">
+        <v>46.55604600796877</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D79" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E79" s="1" t="inlineStr">
+        <is>
+          <t>Joseph HB.mp4</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>1434</v>
+      </c>
+      <c r="G79" t="n">
+        <v>28.500216</v>
+      </c>
+      <c r="H79" t="n">
+        <v>50.31540813585413</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n"/>
+      <c r="B80" s="1" t="n"/>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D80" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E80" s="1" t="inlineStr">
+        <is>
+          <t>Joseph.mp4</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>1450</v>
+      </c>
+      <c r="G80" t="n">
+        <v>28.554858</v>
+      </c>
+      <c r="H80" t="n">
+        <v>50.77945055794009</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n"/>
+      <c r="B81" s="1" t="n"/>
+      <c r="C81" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D81" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E81" s="1" t="inlineStr">
+        <is>
+          <t>Joseph HB.mp4</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>1505</v>
+      </c>
+      <c r="G81" t="n">
+        <v>28.038409</v>
+      </c>
+      <c r="H81" t="n">
+        <v>53.67636944022038</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n"/>
+      <c r="B82" s="1" t="n"/>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D82" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E82" s="1" t="inlineStr">
+        <is>
+          <t>Joseph.mp4</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>1487</v>
+      </c>
+      <c r="G82" t="n">
+        <v>28.196682</v>
+      </c>
+      <c r="H82" t="n">
+        <v>52.73670143175002</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Karlii</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D83" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E83" s="1" t="inlineStr">
+        <is>
+          <t>Karlii HB.mp4</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>2678</v>
+      </c>
+      <c r="G83" t="n">
+        <v>52.347067</v>
+      </c>
+      <c r="H83" t="n">
+        <v>51.15854915042327</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n"/>
+      <c r="B84" s="1" t="n"/>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D84" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E84" s="1" t="inlineStr">
+        <is>
+          <t>Karlii.mp4</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>2642</v>
+      </c>
+      <c r="G84" t="n">
+        <v>52.119155</v>
+      </c>
+      <c r="H84" t="n">
+        <v>50.69153557842601</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n"/>
+      <c r="B85" s="1" t="n"/>
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D85" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E85" s="1" t="inlineStr">
+        <is>
+          <t>Karlii HB.mp4</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>2611</v>
+      </c>
+      <c r="G85" t="n">
+        <v>49.246833</v>
+      </c>
+      <c r="H85" t="n">
+        <v>53.01863776702148</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n"/>
+      <c r="B86" s="1" t="n"/>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D86" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E86" s="1" t="inlineStr">
+        <is>
+          <t>Karlii.mp4</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>2621</v>
+      </c>
+      <c r="G86" t="n">
+        <v>47.38529399999999</v>
+      </c>
+      <c r="H86" t="n">
+        <v>55.31251953401408</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n"/>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D87" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E87" s="1" t="inlineStr">
+        <is>
+          <t>Karlii HB.mp4</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>1505</v>
+      </c>
+      <c r="G87" t="n">
+        <v>33.606376</v>
+      </c>
+      <c r="H87" t="n">
+        <v>44.78316852730566</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n"/>
+      <c r="B88" s="1" t="n"/>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D88" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E88" s="1" t="inlineStr">
+        <is>
+          <t>Karlii.mp4</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>1512</v>
+      </c>
+      <c r="G88" t="n">
+        <v>33.828112</v>
+      </c>
+      <c r="H88" t="n">
+        <v>44.69655297345592</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n"/>
+      <c r="B89" s="1" t="n"/>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D89" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E89" s="1" t="inlineStr">
+        <is>
+          <t>Karlii HB.mp4</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>2981</v>
+      </c>
+      <c r="G89" t="n">
+        <v>56.919398</v>
+      </c>
+      <c r="H89" t="n">
+        <v>52.3723037267541</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n"/>
+      <c r="B90" s="1" t="n"/>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D90" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E90" s="1" t="inlineStr">
+        <is>
+          <t>Karlii.mp4</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>2808</v>
+      </c>
+      <c r="G90" t="n">
+        <v>56.108546</v>
+      </c>
+      <c r="H90" t="n">
+        <v>50.04585219513619</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Kate</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D91" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E91" s="1" t="inlineStr">
+        <is>
+          <t>Kate.mp4</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1278</v>
+      </c>
+      <c r="G91" t="n">
+        <v>21.209762</v>
+      </c>
+      <c r="H91" t="n">
+        <v>60.25527302003672</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n"/>
+      <c r="B92" s="1" t="n"/>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D92" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E92" s="1" t="inlineStr">
+        <is>
+          <t>Kate.mp4</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>1162</v>
+      </c>
+      <c r="G92" t="n">
+        <v>19.262581</v>
+      </c>
+      <c r="H92" t="n">
+        <v>60.32421096632897</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n"/>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D93" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E93" s="1" t="inlineStr">
+        <is>
+          <t>Kate HB.mp4</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>1109</v>
+      </c>
+      <c r="G93" t="n">
+        <v>18.381442</v>
+      </c>
+      <c r="H93" t="n">
+        <v>60.33258979355374</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n"/>
+      <c r="B94" s="1" t="n"/>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D94" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E94" s="1" t="inlineStr">
+        <is>
+          <t>Kate Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>1215</v>
+      </c>
+      <c r="G94" t="n">
+        <v>20.154798</v>
+      </c>
+      <c r="H94" t="n">
+        <v>60.28341241623955</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n"/>
+      <c r="B95" s="1" t="n"/>
+      <c r="C95" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D95" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E95" s="1" t="inlineStr">
+        <is>
+          <t>Kate.mp4</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>1159</v>
+      </c>
+      <c r="G95" t="n">
+        <v>19.22406</v>
+      </c>
+      <c r="H95" t="n">
+        <v>60.28903363805564</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n"/>
+      <c r="B96" s="1" t="n"/>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E96" s="1" t="inlineStr">
+        <is>
+          <t>Kate Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>1194</v>
+      </c>
+      <c r="G96" t="n">
+        <v>19.803892</v>
+      </c>
+      <c r="H96" t="n">
+        <v>60.29117912781992</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D97" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E97" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn HB.mp4</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>1455</v>
+      </c>
+      <c r="G97" t="n">
+        <v>26.482775</v>
+      </c>
+      <c r="H97" t="n">
+        <v>54.94137226933356</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n"/>
+      <c r="B98" s="1" t="n"/>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D98" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E98" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn.mp4</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>1428</v>
+      </c>
+      <c r="G98" t="n">
+        <v>25.753316</v>
+      </c>
+      <c r="H98" t="n">
+        <v>55.44917011851988</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n"/>
+      <c r="B99" s="1" t="n"/>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D99" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E99" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn HB.mp4</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>1547</v>
+      </c>
+      <c r="G99" t="n">
+        <v>32.200929</v>
+      </c>
+      <c r="H99" t="n">
+        <v>48.04209220174983</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n"/>
+      <c r="B100" s="1" t="n"/>
+      <c r="C100" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D100" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E100" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn.mp4</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>1548</v>
+      </c>
+      <c r="G100" t="n">
+        <v>31.544542</v>
+      </c>
+      <c r="H100" t="n">
+        <v>49.07346570446323</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n"/>
+      <c r="B101" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D101" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E101" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn HB.mp4</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>1637</v>
+      </c>
+      <c r="G101" t="n">
+        <v>37.255912</v>
+      </c>
+      <c r="H101" t="n">
+        <v>43.93933505103834</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n"/>
+      <c r="B102" s="1" t="n"/>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D102" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E102" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn.mp4</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>1567</v>
+      </c>
+      <c r="G102" t="n">
+        <v>27.915351</v>
+      </c>
+      <c r="H102" t="n">
+        <v>56.13398878631331</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n"/>
+      <c r="B103" s="1" t="n"/>
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D103" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E103" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn HB.mp4</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>1561</v>
+      </c>
+      <c r="G103" t="n">
+        <v>27.569709</v>
+      </c>
+      <c r="H103" t="n">
+        <v>56.62011158695944</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n"/>
+      <c r="B104" s="1" t="n"/>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D104" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E104" s="1" t="inlineStr">
+        <is>
+          <t>Krystyn.mp4</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>1624</v>
+      </c>
+      <c r="G104" t="n">
+        <v>28.368047</v>
+      </c>
+      <c r="H104" t="n">
+        <v>57.24750808541737</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Melissa</t>
+        </is>
+      </c>
+      <c r="B105" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D105" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E105" s="1" t="inlineStr">
+        <is>
+          <t>Melissa HB.mp4</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>2525</v>
+      </c>
+      <c r="G105" t="n">
+        <v>46.704064</v>
+      </c>
+      <c r="H105" t="n">
+        <v>54.06381765835196</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n"/>
+      <c r="B106" s="1" t="n"/>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D106" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E106" s="1" t="inlineStr">
+        <is>
+          <t>Melissa.mp4</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>3569</v>
+      </c>
+      <c r="G106" t="n">
+        <v>64.145798</v>
+      </c>
+      <c r="H106" t="n">
+        <v>55.63887442790875</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n"/>
+      <c r="B107" s="1" t="n"/>
+      <c r="C107" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D107" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E107" s="1" t="inlineStr">
+        <is>
+          <t>Melissa HB.mp4</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>2786</v>
+      </c>
+      <c r="G107" t="n">
+        <v>57.93909</v>
+      </c>
+      <c r="H107" t="n">
+        <v>48.08498027842688</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n"/>
+      <c r="B108" s="1" t="n"/>
+      <c r="C108" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E108" s="1" t="inlineStr">
+        <is>
+          <t>Melissa.mp4</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>3111</v>
+      </c>
+      <c r="G108" t="n">
+        <v>66.993945</v>
+      </c>
+      <c r="H108" t="n">
+        <v>46.43703248106974</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n"/>
+      <c r="B109" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C109" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D109" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E109" s="1" t="inlineStr">
+        <is>
+          <t>Melissa HB.mp4</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>2606</v>
+      </c>
+      <c r="G109" t="n">
+        <v>50.591942</v>
+      </c>
+      <c r="H109" t="n">
+        <v>51.51017922972792</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n"/>
+      <c r="B110" s="1" t="n"/>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D110" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E110" s="1" t="inlineStr">
+        <is>
+          <t>Melissa.mp4</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>2821</v>
+      </c>
+      <c r="G110" t="n">
+        <v>53.759293</v>
+      </c>
+      <c r="H110" t="n">
+        <v>52.47464842962128</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n"/>
+      <c r="B111" s="1" t="n"/>
+      <c r="C111" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D111" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E111" s="1" t="inlineStr">
+        <is>
+          <t>Melissa HB.mp4</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>2760</v>
+      </c>
+      <c r="G111" t="n">
+        <v>52.458189</v>
+      </c>
+      <c r="H111" t="n">
+        <v>52.61332982730303</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n"/>
+      <c r="B112" s="1" t="n"/>
+      <c r="C112" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D112" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E112" s="1" t="inlineStr">
+        <is>
+          <t>Melissa.mp4</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>2517</v>
+      </c>
+      <c r="G112" t="n">
+        <v>48.236838</v>
+      </c>
+      <c r="H112" t="n">
+        <v>52.18003717407845</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="B113" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C113" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D113" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E113" s="1" t="inlineStr">
+        <is>
+          <t>Nick HB.mp4</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>1352</v>
+      </c>
+      <c r="G113" t="n">
+        <v>34.911123</v>
+      </c>
+      <c r="H113" t="n">
+        <v>38.72691233679306</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n"/>
+      <c r="B114" s="1" t="n"/>
+      <c r="C114" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D114" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E114" s="1" t="inlineStr">
+        <is>
+          <t>Nick.mp4</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>1039</v>
+      </c>
+      <c r="G114" t="n">
+        <v>25.715217</v>
+      </c>
+      <c r="H114" t="n">
+        <v>40.40409225401442</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n"/>
+      <c r="B115" s="1" t="n"/>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D115" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E115" s="1" t="inlineStr">
+        <is>
+          <t>Nick HB.mp4</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>859</v>
+      </c>
+      <c r="G115" t="n">
+        <v>21.460794</v>
+      </c>
+      <c r="H115" t="n">
+        <v>40.02647805109168</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n"/>
+      <c r="B116" s="1" t="n"/>
+      <c r="C116" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D116" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E116" s="1" t="inlineStr">
+        <is>
+          <t>n1.mp4</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>197</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.793938</v>
+      </c>
+      <c r="H116" t="n">
+        <v>34.00105420527455</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n"/>
+      <c r="B117" s="1" t="n"/>
+      <c r="C117" s="1" t="n"/>
+      <c r="D117" s="1" t="n"/>
+      <c r="E117" s="1" t="inlineStr">
+        <is>
+          <t>Nick.mp4</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>2147</v>
+      </c>
+      <c r="G117" t="n">
+        <v>35.730727</v>
+      </c>
+      <c r="H117" t="n">
+        <v>60.08833797308407</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n"/>
+      <c r="B118" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D118" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E118" s="1" t="inlineStr">
+        <is>
+          <t>Nick HB.mp4</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>1306</v>
+      </c>
+      <c r="G118" t="n">
+        <v>25.227786</v>
+      </c>
+      <c r="H118" t="n">
+        <v>51.76831609400841</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n"/>
+      <c r="B119" s="1" t="n"/>
+      <c r="C119" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D119" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E119" s="1" t="inlineStr">
+        <is>
+          <t>Nick.mp4</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>1170</v>
+      </c>
+      <c r="G119" t="n">
+        <v>24.589753</v>
+      </c>
+      <c r="H119" t="n">
+        <v>47.58079513852783</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n"/>
+      <c r="B120" s="1" t="n"/>
+      <c r="C120" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D120" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E120" s="1" t="inlineStr">
+        <is>
+          <t>Nick HB.mp4</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>1173</v>
+      </c>
+      <c r="G120" t="n">
+        <v>24.407189</v>
+      </c>
+      <c r="H120" t="n">
+        <v>48.05961063357194</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n"/>
+      <c r="B121" s="1" t="n"/>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D121" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E121" s="1" t="inlineStr">
+        <is>
+          <t>Nick.mp4</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>1238</v>
+      </c>
+      <c r="G121" t="n">
+        <v>28.231171</v>
+      </c>
+      <c r="H121" t="n">
+        <v>43.85223694759243</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>Rachael B</t>
+        </is>
+      </c>
+      <c r="B122" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C122" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breathe</t>
+        </is>
+      </c>
+      <c r="D122" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E122" s="1" t="inlineStr">
+        <is>
+          <t>Rechael Hold Breathe.mp4</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>1456</v>
+      </c>
+      <c r="G122" t="n">
+        <v>24.173171</v>
+      </c>
+      <c r="H122" t="n">
+        <v>60.23206471339652</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n"/>
+      <c r="B123" s="1" t="n"/>
+      <c r="C123" s="1" t="n"/>
+      <c r="D123" s="1" t="n"/>
+      <c r="E123" s="1" t="inlineStr">
+        <is>
+          <t>Rechael Hold Breathe2.mp4</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>717</v>
+      </c>
+      <c r="G123" t="n">
+        <v>11.858948</v>
+      </c>
+      <c r="H123" t="n">
+        <v>60.46067492664611</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n"/>
+      <c r="B124" s="1" t="n"/>
+      <c r="C124" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D124" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E124" s="1" t="inlineStr">
+        <is>
+          <t>Rachael Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>653</v>
+      </c>
+      <c r="G124" t="n">
+        <v>10.803604</v>
+      </c>
+      <c r="H124" t="n">
+        <v>60.44279297908365</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n"/>
+      <c r="B125" s="1" t="n"/>
+      <c r="C125" s="1" t="n"/>
+      <c r="D125" s="1" t="n"/>
+      <c r="E125" s="1" t="inlineStr">
+        <is>
+          <t>Rachael Relaxed1.mp4</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>731</v>
+      </c>
+      <c r="G125" t="n">
+        <v>12.092245</v>
+      </c>
+      <c r="H125" t="n">
+        <v>60.45196735593763</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n"/>
+      <c r="B126" s="1" t="n"/>
+      <c r="C126" s="1" t="n"/>
+      <c r="D126" s="1" t="n"/>
+      <c r="E126" s="1" t="inlineStr">
+        <is>
+          <t>Rachael Relaxed2.mp4</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>1183</v>
+      </c>
+      <c r="G126" t="n">
+        <v>32.040625</v>
+      </c>
+      <c r="H126" t="n">
+        <v>36.92187652394421</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>Riyan</t>
+        </is>
+      </c>
+      <c r="B127" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C127" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D127" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E127" s="1" t="inlineStr">
+        <is>
+          <t>Riyan HB.mp4</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>1221</v>
+      </c>
+      <c r="G127" t="n">
+        <v>28.050865</v>
+      </c>
+      <c r="H127" t="n">
+        <v>43.52806945525566</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n"/>
+      <c r="B128" s="1" t="n"/>
+      <c r="C128" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D128" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E128" s="1" t="inlineStr">
+        <is>
+          <t>Riyan.mp4</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>1275</v>
+      </c>
+      <c r="G128" t="n">
+        <v>27.371543</v>
+      </c>
+      <c r="H128" t="n">
+        <v>46.58122488746798</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n"/>
+      <c r="B129" s="1" t="n"/>
+      <c r="C129" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D129" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E129" s="1" t="inlineStr">
+        <is>
+          <t>Riyan HB.mp4</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>1442</v>
+      </c>
+      <c r="G129" t="n">
+        <v>27.628191</v>
+      </c>
+      <c r="H129" t="n">
+        <v>52.19306613306676</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n"/>
+      <c r="B130" s="1" t="n"/>
+      <c r="C130" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D130" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E130" s="1" t="inlineStr">
+        <is>
+          <t>Riyan.mp4</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>208</v>
+      </c>
+      <c r="G130" t="n">
+        <v>4.113682</v>
+      </c>
+      <c r="H130" t="n">
+        <v>50.56297496986884</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>Sara</t>
+        </is>
+      </c>
+      <c r="B131" s="1" t="inlineStr">
+        <is>
+          <t>2 Meters</t>
+        </is>
+      </c>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D131" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E131" s="1" t="inlineStr">
+        <is>
+          <t>Sara HB.mp4</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>1328</v>
+      </c>
+      <c r="G131" t="n">
+        <v>22.040165</v>
+      </c>
+      <c r="H131" t="n">
+        <v>60.25363240247975</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n"/>
+      <c r="B132" s="1" t="n"/>
+      <c r="C132" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D132" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E132" s="1" t="inlineStr">
+        <is>
+          <t>Sara Relaxed with Blanket.mp4</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>1451</v>
+      </c>
+      <c r="G132" t="n">
+        <v>24.090906</v>
+      </c>
+      <c r="H132" t="n">
+        <v>60.23019640689312</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n"/>
+      <c r="B133" s="1" t="n"/>
+      <c r="C133" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D133" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E133" s="1" t="inlineStr">
+        <is>
+          <t>Sara Hold Breath.mp4</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>1610</v>
+      </c>
+      <c r="G133" t="n">
+        <v>26.73753</v>
+      </c>
+      <c r="H133" t="n">
+        <v>60.214986201044</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n"/>
+      <c r="B134" s="1" t="n"/>
+      <c r="C134" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D134" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E134" s="1" t="inlineStr">
+        <is>
+          <t>Sara Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>1497</v>
+      </c>
+      <c r="G134" t="n">
+        <v>24.849016</v>
+      </c>
+      <c r="H134" t="n">
+        <v>60.24383420252938</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n"/>
+      <c r="B135" s="1" t="inlineStr">
+        <is>
+          <t>3 Meters</t>
+        </is>
+      </c>
+      <c r="C135" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D135" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E135" s="1" t="inlineStr">
+        <is>
+          <t>Sara HB.mp4</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>1252</v>
+      </c>
+      <c r="G135" t="n">
+        <v>20.772879</v>
+      </c>
+      <c r="H135" t="n">
+        <v>60.27089456401301</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n"/>
+      <c r="B136" s="1" t="n"/>
+      <c r="C136" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D136" s="1" t="inlineStr">
+        <is>
+          <t>With Blankets</t>
+        </is>
+      </c>
+      <c r="E136" s="1" t="inlineStr">
+        <is>
+          <t>Sara Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>1222</v>
+      </c>
+      <c r="G136" t="n">
+        <v>20.266021</v>
+      </c>
+      <c r="H136" t="n">
+        <v>60.29797363774566</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n"/>
+      <c r="B137" s="1" t="n"/>
+      <c r="C137" s="1" t="inlineStr">
+        <is>
+          <t>Hold Breath</t>
+        </is>
+      </c>
+      <c r="D137" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E137" s="1" t="inlineStr">
+        <is>
+          <t>Sara HB.mp4</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>1287</v>
+      </c>
+      <c r="G137" t="n">
+        <v>21.351073</v>
+      </c>
+      <c r="H137" t="n">
+        <v>60.27800101662338</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n"/>
+      <c r="B138" s="1" t="n"/>
+      <c r="C138" s="1" t="inlineStr">
+        <is>
+          <t>Relaxed</t>
+        </is>
+      </c>
+      <c r="D138" s="1" t="inlineStr">
+        <is>
+          <t>Without Blankets</t>
+        </is>
+      </c>
+      <c r="E138" s="1" t="inlineStr">
+        <is>
+          <t>Sara Relaxed.mp4</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>1196</v>
+      </c>
+      <c r="G138" t="n">
+        <v>19.836377</v>
+      </c>
+      <c r="H138" t="n">
+        <v>60.29326827172119</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D27:D28"/>
+  <mergeCells count="70">
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="B131:B134"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="B109:B112"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A20:A29"/>
     <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B46:B49"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="A113:A121"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="B113:B117"/>
     <mergeCell ref="B2:B7"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="B63:B66"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D124:D126"/>
+    <mergeCell ref="A105:A112"/>
+    <mergeCell ref="B118:B121"/>
     <mergeCell ref="A12:A19"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A71:A78"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="A97:A104"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="A20:A27"/>
     <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A127:A130"/>
     <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="A63:A70"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A131:A138"/>
+    <mergeCell ref="C116:C117"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
major refactor to video_to_png
</commit_message>
<xml_diff>
--- a/records/xlsx/rgb.xlsx
+++ b/records/xlsx/rgb.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>frames</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Arun</t>
   </si>
   <si>
-    <t>Illia</t>
-  </si>
-  <si>
     <t>2 Meters</t>
   </si>
   <si>
-    <t>3 Meters</t>
-  </si>
-  <si>
     <t>Hold Breath</t>
   </si>
   <si>
@@ -79,25 +73,7 @@
     <t>relax 2meter short.mp4</t>
   </si>
   <si>
-    <t>Arun3.mp4</t>
-  </si>
-  <si>
-    <t>Illia HB.mp4</t>
-  </si>
-  <si>
-    <t>Illia.mp4</t>
-  </si>
-  <si>
-    <t>Illia HB2.mp4</t>
-  </si>
-  <si>
-    <t>Illia HB1.mp4</t>
-  </si>
-  <si>
     <t>15</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
 </sst>
 </file>
@@ -455,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,28 +471,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F2">
         <v>2146</v>
       </c>
       <c r="G2">
-        <v>73.054497</v>
+        <v>35.76666666666667</v>
       </c>
       <c r="H2">
-        <v>29.37533058368741</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -525,44 +501,44 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>1138</v>
       </c>
       <c r="G3">
-        <v>38.59782</v>
+        <v>18.96666666666667</v>
       </c>
       <c r="H3">
-        <v>29.48353041700283</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F4">
         <v>143</v>
       </c>
       <c r="G4">
-        <v>7.703174999999999</v>
+        <v>2.383333333333333</v>
       </c>
       <c r="H4">
-        <v>18.5637740282416</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -571,437 +547,79 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>1137</v>
       </c>
       <c r="G5">
-        <v>38.190605</v>
+        <v>18.95</v>
       </c>
       <c r="H5">
-        <v>29.77172003428592</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>1790</v>
       </c>
       <c r="G6">
-        <v>36.113806</v>
+        <v>29.83333333333333</v>
       </c>
       <c r="H6">
-        <v>49.56553180797393</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>3872</v>
       </c>
       <c r="G7">
-        <v>72.04854</v>
+        <v>64.53333333333333</v>
       </c>
       <c r="H7">
-        <v>53.74154701816303</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8">
-        <v>1340</v>
-      </c>
-      <c r="G8">
-        <v>37.059608</v>
-      </c>
-      <c r="H8">
-        <v>36.15796475774919</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9">
-        <v>1398</v>
-      </c>
-      <c r="G9">
-        <v>41.309832</v>
-      </c>
-      <c r="H9">
-        <v>33.84182245040358</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10">
-        <v>1438</v>
-      </c>
-      <c r="G10">
-        <v>25.961376</v>
-      </c>
-      <c r="H10">
-        <v>55.38997624779211</v>
-      </c>
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11">
-        <v>1470</v>
-      </c>
-      <c r="G11">
-        <v>26.567759</v>
-      </c>
-      <c r="H11">
-        <v>55.33022186779095</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12">
-        <v>1997</v>
-      </c>
-      <c r="G12">
-        <v>42.697471</v>
-      </c>
-      <c r="H12">
-        <v>46.77091999195924</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13">
-        <v>2311</v>
-      </c>
-      <c r="G13">
-        <v>51.55182600000001</v>
-      </c>
-      <c r="H13">
-        <v>44.82867396394455</v>
-      </c>
-      <c r="I13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14">
-        <v>2154</v>
-      </c>
-      <c r="G14">
-        <v>40.820155</v>
-      </c>
-      <c r="H14">
-        <v>52.76805048878428</v>
-      </c>
-      <c r="I14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>2442</v>
-      </c>
-      <c r="G15">
-        <v>49.465783</v>
-      </c>
-      <c r="H15">
-        <v>49.36745871383457</v>
-      </c>
-      <c r="I15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16">
-        <v>4088</v>
-      </c>
-      <c r="G16">
-        <v>82.335533</v>
-      </c>
-      <c r="H16">
-        <v>49.65049536996378</v>
-      </c>
-      <c r="I16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17">
-        <v>3955</v>
-      </c>
-      <c r="G17">
-        <v>81.783652</v>
-      </c>
-      <c r="H17">
-        <v>48.35929801716362</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18">
-        <v>2808</v>
-      </c>
-      <c r="G18">
-        <v>57.00986900000001</v>
-      </c>
-      <c r="H18">
-        <v>49.25462993082829</v>
-      </c>
-      <c r="I18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19">
-        <v>2290</v>
-      </c>
-      <c r="G19">
-        <v>53.05520600000001</v>
-      </c>
-      <c r="H19">
-        <v>43.16258804084183</v>
-      </c>
-      <c r="I19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20">
-        <v>1740</v>
-      </c>
-      <c r="G20">
-        <v>38.47498</v>
-      </c>
-      <c r="H20">
-        <v>45.22419504831451</v>
-      </c>
-      <c r="I20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21">
-        <v>3071</v>
-      </c>
-      <c r="G21">
-        <v>70.204134</v>
-      </c>
-      <c r="H21">
-        <v>43.74386271896752</v>
-      </c>
-      <c r="I21" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A21"/>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B21"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C19:C20"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>